<commit_message>
Add release 123 archaeal metadata
</commit_message>
<xml_diff>
--- a/data/raw/ExtraCategoriesArchaea.xlsx
+++ b/data/raw/ExtraCategoriesArchaea.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="0" windowWidth="26160" windowHeight="17540" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="998">
   <si>
     <t>0-7.5 cm soil sample from a meadow incubated as anoxic slurry</t>
   </si>
@@ -2278,6 +2278,741 @@
   </si>
   <si>
     <t>ZN</t>
+  </si>
+  <si>
+    <t>10-20 meters below sea level off the coast of Santa Barbara, CA, USA</t>
+  </si>
+  <si>
+    <t>10% Pt methanogenic biocathode</t>
+  </si>
+  <si>
+    <t>A pilot-scale bioreactor, BRGM, France</t>
+  </si>
+  <si>
+    <t>abomasum</t>
+  </si>
+  <si>
+    <t>acid hot spring</t>
+  </si>
+  <si>
+    <t>Acid Mine Los Rueldos</t>
+  </si>
+  <si>
+    <t>acid sulfate soils</t>
+  </si>
+  <si>
+    <t>acidic paddy soil</t>
+  </si>
+  <si>
+    <t>Adriatic sea</t>
+  </si>
+  <si>
+    <t>alpine lake sediment</t>
+  </si>
+  <si>
+    <t>anaerobic bioreactor for auto-generative high pressure digestion</t>
+  </si>
+  <si>
+    <t>anaerobic, low pH pit mud of Luzhou-flavor liquor</t>
+  </si>
+  <si>
+    <t>anode biofilm in microbial fuel cells</t>
+  </si>
+  <si>
+    <t>Aran-Bidgol salt lake</t>
+  </si>
+  <si>
+    <t>Ayakekum salt lake - low temperature, low nutrient levels, abundant sunlight and remote geographical location; pH of the water was approximately pH 7-8</t>
+  </si>
+  <si>
+    <t>Ayakekumsalt Lake</t>
+  </si>
+  <si>
+    <t>Baltic Sea Thaumarchaeota enrichment culture</t>
+  </si>
+  <si>
+    <t>Banaskatha coal mine</t>
+  </si>
+  <si>
+    <t>base of Lung Snack Piccard Beebee Woods Mound Mid Cayman Rise</t>
+  </si>
+  <si>
+    <t>biofilm from subsurface sulfidic cave stream</t>
+  </si>
+  <si>
+    <t>biogas treated cow ding</t>
+  </si>
+  <si>
+    <t>bioleaching process</t>
+  </si>
+  <si>
+    <t>biomass at the Mediterranean DCM (50m)</t>
+  </si>
+  <si>
+    <t>Black Sea salt</t>
+  </si>
+  <si>
+    <t>Black smoker chimney at the Kairei field in the Central Indian Ridge</t>
+  </si>
+  <si>
+    <t>body brine (salinity 120g/L) of Thetis anoxic lake 3500m, Southern Ionian Sea</t>
+  </si>
+  <si>
+    <t>body brine (salinity 220g/L) of Thetis anoxic lake 3500m, Southern Ionian Sea</t>
+  </si>
+  <si>
+    <t>Bolivian salt</t>
+  </si>
+  <si>
+    <t>Brancoveanu lake</t>
+  </si>
+  <si>
+    <t>Brazilian Caatinga soil</t>
+  </si>
+  <si>
+    <t>Brine</t>
+  </si>
+  <si>
+    <t>brine from hypersaline Lake Medee</t>
+  </si>
+  <si>
+    <t>brine sample</t>
+  </si>
+  <si>
+    <t>brine sample from Aran-Bidgol salt lake</t>
+  </si>
+  <si>
+    <t>brine sample from salt lake</t>
+  </si>
+  <si>
+    <t>Brine-seawater interface of Atlantis II Deep, Red Sea</t>
+  </si>
+  <si>
+    <t>Brine-seawater interface of Discovery Deep, Red Sea</t>
+  </si>
+  <si>
+    <t>Brine-seawater interface of Erba Deep, Red Sea</t>
+  </si>
+  <si>
+    <t>Brine-seawater interface of Kebrit Deep, Red Sea</t>
+  </si>
+  <si>
+    <t>Brine-seawater interface of Nereus Deep, Red Sea</t>
+  </si>
+  <si>
+    <t>Camargue salt</t>
+  </si>
+  <si>
+    <t>cellulose anaerobic digester</t>
+  </si>
+  <si>
+    <t>Chardonnay salt</t>
+  </si>
+  <si>
+    <t>Cistern Spring (CIS_19); temperature 78C; pH 4.4</t>
+  </si>
+  <si>
+    <t>clay from marine sediments 136 meters below sea floor depth collected from drilling site U1352C during the IODP 317 cruise</t>
+  </si>
+  <si>
+    <t>clay from marine sediments 31 meters below sea floor depth collected from drilling site U1352C during the IODP 317 cruise</t>
+  </si>
+  <si>
+    <t>clone from PCR product of water sample</t>
+  </si>
+  <si>
+    <t>coastal surface water from the Northern Adriatic Sea</t>
+  </si>
+  <si>
+    <t>coastal/estuarine sediments</t>
+  </si>
+  <si>
+    <t>colonic digesta of grown pigs</t>
+  </si>
+  <si>
+    <t>colonic digesta of young pigs</t>
+  </si>
+  <si>
+    <t>colonic mucosa of grown pigs</t>
+  </si>
+  <si>
+    <t>column bioleaching</t>
+  </si>
+  <si>
+    <t>combined biofilm from UBA (pink subaerial biofilm) and UBA BS (thick floating biofilm subdivided into strips) samples</t>
+  </si>
+  <si>
+    <t>commercial biogas plant</t>
+  </si>
+  <si>
+    <t>constructed wetland for wastewater treatment</t>
+  </si>
+  <si>
+    <t>Copahue geotherma field, Neuquen, Argentina</t>
+  </si>
+  <si>
+    <t>Crater Hills, Alice Spring (CH-AS); temperature 75C; pH 2.5</t>
+  </si>
+  <si>
+    <t>Dabancheng salt lake</t>
+  </si>
+  <si>
+    <t>deep sea surface sediment</t>
+  </si>
+  <si>
+    <t>dental human plaque of periodontitis patients</t>
+  </si>
+  <si>
+    <t>derived from human gut metagenome</t>
+  </si>
+  <si>
+    <t>discovery brine interface of Red Sea</t>
+  </si>
+  <si>
+    <t>Drake Passage</t>
+  </si>
+  <si>
+    <t>East Pacific Ridge</t>
+  </si>
+  <si>
+    <t>Eastern Lau Spreading Center</t>
+  </si>
+  <si>
+    <t>Eel River Basin carbonate 2688</t>
+  </si>
+  <si>
+    <t>Eel River Basin sediment 2688</t>
+  </si>
+  <si>
+    <t>Eel River sediment</t>
+  </si>
+  <si>
+    <t>enrichment culture fed with acetate and methanol at 35 degrees in a sequencing batch reactor (SBR)</t>
+  </si>
+  <si>
+    <t>enrichment fermentation of pig feces with beta-glucan substrate</t>
+  </si>
+  <si>
+    <t>enrichment fermentation of pig feces without beta-glucan substrate</t>
+  </si>
+  <si>
+    <t>evaporitic salt crystal</t>
+  </si>
+  <si>
+    <t>extreme hypersaline lake water from Lake Tyrrell</t>
+  </si>
+  <si>
+    <t>extremely saline anoxic brine of the deep-sea hypersaline anoxic lake (DHAL) Thetis located South-East of the Medriff corridor collected during oceanographic cruises of the RV Urania in September 2009</t>
+  </si>
+  <si>
+    <t>Fara Fund lake</t>
+  </si>
+  <si>
+    <t>feces; sample TS28</t>
+  </si>
+  <si>
+    <t>feces; sample TS29</t>
+  </si>
+  <si>
+    <t>fermentative hydrogen production biomass</t>
+  </si>
+  <si>
+    <t>filtered surface water from Lake Tyrrell</t>
+  </si>
+  <si>
+    <t>freshwater fish tank</t>
+  </si>
+  <si>
+    <t>freshwater hot-pool in Kuirau Park</t>
+  </si>
+  <si>
+    <t>freshwater lake sediment grown in bioreactor fed with nitrate, ammonium and methane</t>
+  </si>
+  <si>
+    <t>fumarolic soil at 65 degrees C, pH8</t>
+  </si>
+  <si>
+    <t>Gangxi solar saltern, an artificial marine solar saltern</t>
+  </si>
+  <si>
+    <t>Gozo Island salt</t>
+  </si>
+  <si>
+    <t>granular sludge from a brewing industry</t>
+  </si>
+  <si>
+    <t>graphite block methanogenic biocathode</t>
+  </si>
+  <si>
+    <t>Guaymas Basin</t>
+  </si>
+  <si>
+    <t>Guaymas Basin Hydrothermal Plumes and Background; water depths 1600, 1775, 1900, 1996 m</t>
+  </si>
+  <si>
+    <t>Guerande salt</t>
+  </si>
+  <si>
+    <t>Gulf of Maine surface waters</t>
+  </si>
+  <si>
+    <t>Gulf of Mexico, Mississippi Canyon, MC118, sediments</t>
+  </si>
+  <si>
+    <t>Halen Mon salt</t>
+  </si>
+  <si>
+    <t>Halophytes</t>
+  </si>
+  <si>
+    <t>Himalayan pink salt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hot cracks </t>
+  </si>
+  <si>
+    <t>hot marine sediment</t>
+  </si>
+  <si>
+    <t>Hot spring</t>
+  </si>
+  <si>
+    <t>Hot spring in Mutnovsky Volcano</t>
+  </si>
+  <si>
+    <t>hot spring water and gravel</t>
+  </si>
+  <si>
+    <t>hot springs at Los Azufres National Park</t>
+  </si>
+  <si>
+    <t>human brain abscess</t>
+  </si>
+  <si>
+    <t>human stool specimen</t>
+  </si>
+  <si>
+    <t>Hydrate Ridge carbonate 2518</t>
+  </si>
+  <si>
+    <t>Hydrate Ridge sediment 2518</t>
+  </si>
+  <si>
+    <t>Hydrate Ridge, OR</t>
+  </si>
+  <si>
+    <t>hydrocarbon-contaminated sediment, Bemidji core 1110</t>
+  </si>
+  <si>
+    <t>hydrothermal carbonate rock</t>
+  </si>
+  <si>
+    <t>hydrothermal plume and surrounding water mass above the active hydrothermal field of the Southwest Indian Ridge</t>
+  </si>
+  <si>
+    <t>hypermesophilic terephthalate degrading bioreactor</t>
+  </si>
+  <si>
+    <t>hypersaline chloride sulfate lake of Kulunda Steppe</t>
+  </si>
+  <si>
+    <t>hypersaline endoevaporitic microbial mat</t>
+  </si>
+  <si>
+    <t>Hypersaline microbial mat</t>
+  </si>
+  <si>
+    <t>hypersaline produced water from the campos basin</t>
+  </si>
+  <si>
+    <t>hypersaline sample from solar saltern, pond crsytalizer CR30</t>
+  </si>
+  <si>
+    <t>hypersaline spring</t>
+  </si>
+  <si>
+    <t>hypersaline water sample from Lake Tyrrell</t>
+  </si>
+  <si>
+    <t>hypersaline waters of Lake Tyrrell</t>
+  </si>
+  <si>
+    <t>interface from Kryos DHAL 3337m</t>
+  </si>
+  <si>
+    <t>Ionian sea</t>
+  </si>
+  <si>
+    <t>iron corrossion-inducing microbial community</t>
+  </si>
+  <si>
+    <t>isolated as part of a large dataset composed predominantly from surface water marine samples collected along a voyage from Eastern North American coast to the Eastern Pacific Ocean, including locations in the Sargasso Sea, Panama Canal, and the Galapagos Islands</t>
+  </si>
+  <si>
+    <t>Joseph's Coat Hot Spring, Scorodite Spring (JC3A); temperature 80C; pH 6.1</t>
+  </si>
+  <si>
+    <t>La Palma Flor de Sal</t>
+  </si>
+  <si>
+    <t>lab scale mesophilic 35 C anaerobic semi-continuous digesters fed with dairy farm wastes</t>
+  </si>
+  <si>
+    <t>Lac Rose salt</t>
+  </si>
+  <si>
+    <t>Lake Tyrrell</t>
+  </si>
+  <si>
+    <t>lowermost (B1B) sediment-attached strata from acid streamer/mats thriving at Los Rueldos abandoned Hg mine</t>
+  </si>
+  <si>
+    <t>Maras salt</t>
+  </si>
+  <si>
+    <t>Marine bioreactor</t>
+  </si>
+  <si>
+    <t>marine oilfield, North sea</t>
+  </si>
+  <si>
+    <t>Marine sediment from Hiroshima Bay</t>
+  </si>
+  <si>
+    <t>marine sediment taken 10 cm below seafloor</t>
+  </si>
+  <si>
+    <t>Marker113 at caldera of Axial Seamount</t>
+  </si>
+  <si>
+    <t>mesophilic (35oC) anaerobic digesters fed by diary farm waste</t>
+  </si>
+  <si>
+    <t>BDBD</t>
+  </si>
+  <si>
+    <t>mesophilic anaerobic digester treating municipal wastewater sludge</t>
+  </si>
+  <si>
+    <t>Metagenomic fosmid libraries constructed from a methanotrophic microbial mat growing in the Black Sea</t>
+  </si>
+  <si>
+    <t>Methane hydrate sediment</t>
+  </si>
+  <si>
+    <t>mine environment soil</t>
+  </si>
+  <si>
+    <t>mixture of activated sludge and methanogenic sludge; day 435</t>
+  </si>
+  <si>
+    <t>mud of drilling swamp</t>
+  </si>
+  <si>
+    <t>mud sample collected next to a hot spring at the Los Azufres geothermal field</t>
+  </si>
+  <si>
+    <t>natural gas-associated formation water in aquifers</t>
+  </si>
+  <si>
+    <t>Norris Geyser Basin, Beowulf Spring (NGB-BED); temperature 65C; pH 3.0</t>
+  </si>
+  <si>
+    <t>Nyegga cold-seep field located at the mid-Norwegian margin on the northern edge of the Storegga Slide</t>
+  </si>
+  <si>
+    <t>Ocean drilling core sample</t>
+  </si>
+  <si>
+    <t>Ocean water at 3 m depth at station HL4 from Atlantic Zone Monitoring Program (AZMP)</t>
+  </si>
+  <si>
+    <t>Ocnei Lake</t>
+  </si>
+  <si>
+    <t>oil field water</t>
+  </si>
+  <si>
+    <t>oil formation water</t>
+  </si>
+  <si>
+    <t>Oil sands tailings enrichment culture</t>
+  </si>
+  <si>
+    <t>oil-field</t>
+  </si>
+  <si>
+    <t>oil-immersed sample from Guaymas Basin</t>
+  </si>
+  <si>
+    <t>Pakistani rock salt</t>
+  </si>
+  <si>
+    <t>Persian blue rock salt</t>
+  </si>
+  <si>
+    <t>pink biofilm microbial community collected from flowing acid mine drainage (pH 0.8, 42C)</t>
+  </si>
+  <si>
+    <t>plumage</t>
+  </si>
+  <si>
+    <t>Qi'ao Island</t>
+  </si>
+  <si>
+    <t>Qinshui basin coalbed water</t>
+  </si>
+  <si>
+    <t>raw salt</t>
+  </si>
+  <si>
+    <t>AQR</t>
+  </si>
+  <si>
+    <t>reed roots from a constructed wetland</t>
+  </si>
+  <si>
+    <t>refuse dump Nest 11 layer 3</t>
+  </si>
+  <si>
+    <t>refuse dump Nest 12 layer 0</t>
+  </si>
+  <si>
+    <t>refuse dump Nest 12 layer 1</t>
+  </si>
+  <si>
+    <t>refuse dump Nest 12 layer 2</t>
+  </si>
+  <si>
+    <t>refuse dump Nest 12 layer 4</t>
+  </si>
+  <si>
+    <t>refuse dump Nest 9 layer 0</t>
+  </si>
+  <si>
+    <t>refuse dump Nest 9 layer 2</t>
+  </si>
+  <si>
+    <t>refuse dump Nest 9 layer 4</t>
+  </si>
+  <si>
+    <t>rhizosphere of Abutilon</t>
+  </si>
+  <si>
+    <t>rhizosphere of Banni grass</t>
+  </si>
+  <si>
+    <t>rhizosphere of Cenchrus setigerus</t>
+  </si>
+  <si>
+    <t>rhizosphere of Cressa cretica</t>
+  </si>
+  <si>
+    <t>rhizosphere of Dicanthium</t>
+  </si>
+  <si>
+    <t>rhizosphere of Oain plant</t>
+  </si>
+  <si>
+    <t>rhizosphere of plant of Asteraceae family</t>
+  </si>
+  <si>
+    <t>rhizosphere of Sporobolus</t>
+  </si>
+  <si>
+    <t>rhizosphere of Suaeda nudiflora</t>
+  </si>
+  <si>
+    <t>Rifle groundwater metagenome at time 1 / A; 0.2 micron filter</t>
+  </si>
+  <si>
+    <t>rock salt drill core samples from the depth of ~800 m, Yunying salt mine</t>
+  </si>
+  <si>
+    <t>rumen fluid of Dechang buffalo</t>
+  </si>
+  <si>
+    <t>rumen fluid of Dechang buffalorumen fluid of Dechang buffalorumen fluid of Dechang buffalo</t>
+  </si>
+  <si>
+    <t>rumen fluid of water buffalo</t>
+  </si>
+  <si>
+    <t>rumen fluid of water buffalo in China</t>
+  </si>
+  <si>
+    <t>rumen methanogens from Budorcas taxicolor bedfordi</t>
+  </si>
+  <si>
+    <t>saline soil from Tarim Basin</t>
+  </si>
+  <si>
+    <t>salt crystallizer Little Rann of Kutch</t>
+  </si>
+  <si>
+    <t>Salt Crystallizer Pond</t>
+  </si>
+  <si>
+    <t>salt crystallizer pond</t>
+  </si>
+  <si>
+    <t>salt lake sediments</t>
+  </si>
+  <si>
+    <t>saltern pond</t>
+  </si>
+  <si>
+    <t>Saltern solar multipond</t>
+  </si>
+  <si>
+    <t>seawater filtered on 0.2 um membrane filter at a depth of 60m, temperature: 13.53 celsius degree, salinity: 34.85, dissolved oxygen concentration:1.8 uM</t>
+  </si>
+  <si>
+    <t>sediment associated with methane hydrate from Krishna Godavari Basin</t>
+  </si>
+  <si>
+    <t>sediment from saline lake</t>
+  </si>
+  <si>
+    <t>sediment of pond</t>
+  </si>
+  <si>
+    <t>sediment of reec</t>
+  </si>
+  <si>
+    <t>sediment of reed</t>
+  </si>
+  <si>
+    <t>sediment-brine interface of the Shaban Deep in the Red Sea</t>
+  </si>
+  <si>
+    <t>sediments from an inland lake</t>
+  </si>
+  <si>
+    <t>Sheyang marine solar saltern</t>
+  </si>
+  <si>
+    <t>single cell amplified by MDA; Atlantis II deep Red Sea brine-seawater interface</t>
+  </si>
+  <si>
+    <t>single cell amplified by MDA; Atlantis II Deep Red Sea brine-seawater interface</t>
+  </si>
+  <si>
+    <t>sludge from full-scale UASB reactor treating PTA wastewater</t>
+  </si>
+  <si>
+    <t>sludge layer in laboratory-scale septic tanks</t>
+  </si>
+  <si>
+    <t>soil aquifer system</t>
+  </si>
+  <si>
+    <t>soil from saline lake</t>
+  </si>
+  <si>
+    <t>soil sample from Sambhar lake</t>
+  </si>
+  <si>
+    <t>Solar salt</t>
+  </si>
+  <si>
+    <t>solar saltern at 12% salinity</t>
+  </si>
+  <si>
+    <t>solar saltern from Mohei salt mine</t>
+  </si>
+  <si>
+    <t>solar saltern water</t>
+  </si>
+  <si>
+    <t>South Atlantic</t>
+  </si>
+  <si>
+    <t>spring saltern</t>
+  </si>
+  <si>
+    <t>sub-cultured for isolation from anaerobic microbial enrichment culture derived from a coal seam gas formation water sample</t>
+  </si>
+  <si>
+    <t>submarine canyon sediments off the coast of southern California</t>
+  </si>
+  <si>
+    <t>submerged non-stratified mat biofilm (B2A) from acid streamer/mats thriving at Los Rueldos abandoned Hg mine</t>
+  </si>
+  <si>
+    <t>sulfide rock in a flange from Godzilla, an active hydrothermal vent sulfide chimney in the High Rise Hydrothermal vent field (at 47 58.00'N and 129 05.50'W), along the Endeavour segment of the Juan de Fuca Ridge, at a depth of 2144 m, approximately 300 miles west of Seattle, in the Northeast Pacific Ocean</t>
+  </si>
+  <si>
+    <t>sulfidic aquifer Muehlbacher Schwefelquelle</t>
+  </si>
+  <si>
+    <t>sulfidic groundwater</t>
+  </si>
+  <si>
+    <t>sulfur and silica sinter at air/water interface</t>
+  </si>
+  <si>
+    <t>surficial sediments beneath a 12-ft water column from coastal/estuarine sediments</t>
+  </si>
+  <si>
+    <t>thermal and acidic green biofilms from a fumarole</t>
+  </si>
+  <si>
+    <t>thermal soil</t>
+  </si>
+  <si>
+    <t>thermophilic electromethanogenic bioelectrochemical reactor biocathode</t>
+  </si>
+  <si>
+    <t>thermophilic sludge anaerobic digestion</t>
+  </si>
+  <si>
+    <t>total DNA isolated from fresh water sediment, Nov. 2003, Orsay, France</t>
+  </si>
+  <si>
+    <t>Traditional salt-fermented seafood in Korea</t>
+  </si>
+  <si>
+    <t>transitional zone</t>
+  </si>
+  <si>
+    <t>two 30-60 cm subsurface water samples (65C) from the hot springs at Los Azufres National Park</t>
+  </si>
+  <si>
+    <t>UAFB system treated with terephthalate contained wastewater</t>
+  </si>
+  <si>
+    <t>Upper convective layer of Atlantis II Deep, Red Sea</t>
+  </si>
+  <si>
+    <t>walls of a black smoker at a deep-sea hydrothermal vent, 9</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>water from hydrothermal chimney-like structure</t>
+  </si>
+  <si>
+    <t>White Rann soil</t>
+  </si>
+  <si>
+    <t>White Rann water</t>
+  </si>
+  <si>
+    <t>Yangjiang marine solar saltern</t>
+  </si>
+  <si>
+    <t>yellow water of Chinese intense flavor liquor cellar</t>
+  </si>
+  <si>
+    <t>Yinggehai marine solar saltern</t>
+  </si>
+  <si>
+    <t>Zara Saltern, Sivas (spring saltern)</t>
+  </si>
+  <si>
+    <t>Zhoushan marine solar saltern</t>
   </si>
 </sst>
 </file>
@@ -2858,15 +3593,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B727"/>
+  <dimension ref="A1:B970"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A420" workbookViewId="0">
+      <selection activeCell="B440" sqref="B440"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="122.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8684,6 +9419,1950 @@
       </c>
       <c r="B727" t="s">
         <v>743</v>
+      </c>
+    </row>
+    <row r="728" spans="1:2">
+      <c r="A728" t="s">
+        <v>3</v>
+      </c>
+      <c r="B728" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="729" spans="1:2">
+      <c r="A729" t="s">
+        <v>10</v>
+      </c>
+      <c r="B729" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="730" spans="1:2">
+      <c r="A730" t="s">
+        <v>10</v>
+      </c>
+      <c r="B730" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="731" spans="1:2">
+      <c r="A731" t="s">
+        <v>70</v>
+      </c>
+      <c r="B731" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="732" spans="1:2">
+      <c r="A732" t="s">
+        <v>8</v>
+      </c>
+      <c r="B732" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="733" spans="1:2">
+      <c r="A733" t="s">
+        <v>745</v>
+      </c>
+      <c r="B733" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="734" spans="1:2">
+      <c r="A734" t="s">
+        <v>1</v>
+      </c>
+      <c r="B734" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="735" spans="1:2">
+      <c r="A735" t="s">
+        <v>1</v>
+      </c>
+      <c r="B735" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="736" spans="1:2">
+      <c r="A736" t="s">
+        <v>3</v>
+      </c>
+      <c r="B736" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="737" spans="1:2">
+      <c r="A737" t="s">
+        <v>183</v>
+      </c>
+      <c r="B737" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="738" spans="1:2">
+      <c r="A738" t="s">
+        <v>10</v>
+      </c>
+      <c r="B738" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="739" spans="1:2">
+      <c r="A739" t="s">
+        <v>183</v>
+      </c>
+      <c r="B739" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="740" spans="1:2">
+      <c r="A740" t="s">
+        <v>10</v>
+      </c>
+      <c r="B740" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="741" spans="1:2">
+      <c r="A741" t="s">
+        <v>3</v>
+      </c>
+      <c r="B741" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="742" spans="1:2">
+      <c r="A742" t="s">
+        <v>3</v>
+      </c>
+      <c r="B742" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="743" spans="1:2">
+      <c r="A743" t="s">
+        <v>3</v>
+      </c>
+      <c r="B743" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="744" spans="1:2">
+      <c r="A744" t="s">
+        <v>3</v>
+      </c>
+      <c r="B744" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="745" spans="1:2">
+      <c r="A745" t="s">
+        <v>745</v>
+      </c>
+      <c r="B745" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="746" spans="1:2">
+      <c r="A746" t="s">
+        <v>8</v>
+      </c>
+      <c r="B746" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="747" spans="1:2">
+      <c r="A747" t="s">
+        <v>1</v>
+      </c>
+      <c r="B747" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="748" spans="1:2">
+      <c r="A748" t="s">
+        <v>10</v>
+      </c>
+      <c r="B748" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="749" spans="1:2">
+      <c r="A749" t="s">
+        <v>10</v>
+      </c>
+      <c r="B749" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="750" spans="1:2">
+      <c r="A750" t="s">
+        <v>3</v>
+      </c>
+      <c r="B750" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="751" spans="1:2">
+      <c r="A751" t="s">
+        <v>1</v>
+      </c>
+      <c r="B751" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="752" spans="1:2">
+      <c r="A752" t="s">
+        <v>8</v>
+      </c>
+      <c r="B752" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="753" spans="1:2">
+      <c r="A753" t="s">
+        <v>242</v>
+      </c>
+      <c r="B753" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="754" spans="1:2">
+      <c r="A754" t="s">
+        <v>242</v>
+      </c>
+      <c r="B754" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="755" spans="1:2">
+      <c r="A755" t="s">
+        <v>1</v>
+      </c>
+      <c r="B755" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="756" spans="1:2">
+      <c r="A756" t="s">
+        <v>55</v>
+      </c>
+      <c r="B756" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="757" spans="1:2">
+      <c r="A757" t="s">
+        <v>1</v>
+      </c>
+      <c r="B757" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="758" spans="1:2">
+      <c r="A758" t="s">
+        <v>242</v>
+      </c>
+      <c r="B758" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="759" spans="1:2">
+      <c r="A759" t="s">
+        <v>242</v>
+      </c>
+      <c r="B759" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="760" spans="1:2">
+      <c r="A760" t="s">
+        <v>242</v>
+      </c>
+      <c r="B760" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="761" spans="1:2">
+      <c r="A761" t="s">
+        <v>242</v>
+      </c>
+      <c r="B761" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="762" spans="1:2">
+      <c r="A762" t="s">
+        <v>242</v>
+      </c>
+      <c r="B762" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="763" spans="1:2">
+      <c r="A763" t="s">
+        <v>242</v>
+      </c>
+      <c r="B763" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="764" spans="1:2">
+      <c r="A764" t="s">
+        <v>242</v>
+      </c>
+      <c r="B764" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="765" spans="1:2">
+      <c r="A765" t="s">
+        <v>242</v>
+      </c>
+      <c r="B765" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="766" spans="1:2">
+      <c r="A766" t="s">
+        <v>242</v>
+      </c>
+      <c r="B766" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="767" spans="1:2">
+      <c r="A767" t="s">
+        <v>242</v>
+      </c>
+      <c r="B767" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="768" spans="1:2">
+      <c r="A768" t="s">
+        <v>1</v>
+      </c>
+      <c r="B768" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="769" spans="1:2">
+      <c r="A769" t="s">
+        <v>10</v>
+      </c>
+      <c r="B769" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="770" spans="1:2">
+      <c r="A770" t="s">
+        <v>1</v>
+      </c>
+      <c r="B770" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="771" spans="1:2">
+      <c r="A771" t="s">
+        <v>8</v>
+      </c>
+      <c r="B771" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="772" spans="1:2">
+      <c r="A772" t="s">
+        <v>6</v>
+      </c>
+      <c r="B772" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="773" spans="1:2">
+      <c r="A773" t="s">
+        <v>6</v>
+      </c>
+      <c r="B773" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="774" spans="1:2">
+      <c r="A774" t="s">
+        <v>423</v>
+      </c>
+      <c r="B774" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="775" spans="1:2">
+      <c r="A775" t="s">
+        <v>3</v>
+      </c>
+      <c r="B775" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="776" spans="1:2">
+      <c r="A776" t="s">
+        <v>210</v>
+      </c>
+      <c r="B776" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="777" spans="1:2">
+      <c r="A777" t="s">
+        <v>70</v>
+      </c>
+      <c r="B777" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="778" spans="1:2">
+      <c r="A778" t="s">
+        <v>70</v>
+      </c>
+      <c r="B778" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="779" spans="1:2">
+      <c r="A779" t="s">
+        <v>70</v>
+      </c>
+      <c r="B779" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="780" spans="1:2">
+      <c r="A780" t="s">
+        <v>745</v>
+      </c>
+      <c r="B780" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="781" spans="1:2">
+      <c r="A781" t="s">
+        <v>10</v>
+      </c>
+      <c r="B781" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="782" spans="1:2">
+      <c r="A782" t="s">
+        <v>10</v>
+      </c>
+      <c r="B782" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="783" spans="1:2">
+      <c r="A783" t="s">
+        <v>10</v>
+      </c>
+      <c r="B783" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="784" spans="1:2">
+      <c r="A784" t="s">
+        <v>8</v>
+      </c>
+      <c r="B784" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="785" spans="1:2">
+      <c r="A785" t="s">
+        <v>8</v>
+      </c>
+      <c r="B785" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="786" spans="1:2">
+      <c r="A786" t="s">
+        <v>3</v>
+      </c>
+      <c r="B786" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="787" spans="1:2">
+      <c r="A787" t="s">
+        <v>6</v>
+      </c>
+      <c r="B787" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="788" spans="1:2">
+      <c r="A788" t="s">
+        <v>70</v>
+      </c>
+      <c r="B788" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="789" spans="1:2">
+      <c r="A789" t="s">
+        <v>70</v>
+      </c>
+      <c r="B789" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="790" spans="1:2">
+      <c r="A790" t="s">
+        <v>242</v>
+      </c>
+      <c r="B790" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="791" spans="1:2">
+      <c r="A791" t="s">
+        <v>3</v>
+      </c>
+      <c r="B791" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="792" spans="1:2">
+      <c r="A792" t="s">
+        <v>6</v>
+      </c>
+      <c r="B792" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="793" spans="1:2">
+      <c r="A793" t="s">
+        <v>6</v>
+      </c>
+      <c r="B793" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="794" spans="1:2">
+      <c r="A794" t="s">
+        <v>183</v>
+      </c>
+      <c r="B794" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="795" spans="1:2">
+      <c r="A795" t="s">
+        <v>183</v>
+      </c>
+      <c r="B795" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="796" spans="1:2">
+      <c r="A796" t="s">
+        <v>183</v>
+      </c>
+      <c r="B796" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="797" spans="1:2">
+      <c r="A797" t="s">
+        <v>10</v>
+      </c>
+      <c r="B797" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="798" spans="1:2">
+      <c r="A798" t="s">
+        <v>10</v>
+      </c>
+      <c r="B798" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="799" spans="1:2">
+      <c r="A799" t="s">
+        <v>70</v>
+      </c>
+      <c r="B799" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="800" spans="1:2">
+      <c r="A800" t="s">
+        <v>1</v>
+      </c>
+      <c r="B800" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="801" spans="1:2">
+      <c r="A801" t="s">
+        <v>3</v>
+      </c>
+      <c r="B801" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="802" spans="1:2">
+      <c r="A802" t="s">
+        <v>242</v>
+      </c>
+      <c r="B802" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="803" spans="1:2">
+      <c r="A803" t="s">
+        <v>55</v>
+      </c>
+      <c r="B803" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="804" spans="1:2">
+      <c r="A804" t="s">
+        <v>70</v>
+      </c>
+      <c r="B804" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="805" spans="1:2">
+      <c r="A805" t="s">
+        <v>70</v>
+      </c>
+      <c r="B805" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="806" spans="1:2">
+      <c r="A806" t="s">
+        <v>10</v>
+      </c>
+      <c r="B806" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="807" spans="1:2">
+      <c r="A807" t="s">
+        <v>55</v>
+      </c>
+      <c r="B807" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="808" spans="1:2">
+      <c r="A808" t="s">
+        <v>423</v>
+      </c>
+      <c r="B808" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="809" spans="1:2">
+      <c r="A809" t="s">
+        <v>8</v>
+      </c>
+      <c r="B809" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="810" spans="1:2">
+      <c r="A810" t="s">
+        <v>10</v>
+      </c>
+      <c r="B810" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="811" spans="1:2">
+      <c r="A811" t="s">
+        <v>1</v>
+      </c>
+      <c r="B811" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="812" spans="1:2">
+      <c r="A812" t="s">
+        <v>3</v>
+      </c>
+      <c r="B812" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="813" spans="1:2">
+      <c r="A813" t="s">
+        <v>1</v>
+      </c>
+      <c r="B813" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="814" spans="1:2">
+      <c r="A814" t="s">
+        <v>10</v>
+      </c>
+      <c r="B814" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="815" spans="1:2">
+      <c r="A815" t="s">
+        <v>10</v>
+      </c>
+      <c r="B815" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="816" spans="1:2">
+      <c r="A816" t="s">
+        <v>6</v>
+      </c>
+      <c r="B816" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="817" spans="1:2">
+      <c r="A817" t="s">
+        <v>8</v>
+      </c>
+      <c r="B817" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="818" spans="1:2">
+      <c r="A818" t="s">
+        <v>1</v>
+      </c>
+      <c r="B818" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="819" spans="1:2">
+      <c r="A819" t="s">
+        <v>3</v>
+      </c>
+      <c r="B819" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="820" spans="1:2">
+      <c r="A820" t="s">
+        <v>6</v>
+      </c>
+      <c r="B820" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="821" spans="1:2">
+      <c r="A821" t="s">
+        <v>1</v>
+      </c>
+      <c r="B821" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="822" spans="1:2">
+      <c r="A822" t="s">
+        <v>3</v>
+      </c>
+      <c r="B822" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="823" spans="1:2">
+      <c r="A823" t="s">
+        <v>1</v>
+      </c>
+      <c r="B823" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="824" spans="1:2">
+      <c r="A824" t="s">
+        <v>8</v>
+      </c>
+      <c r="B824" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="825" spans="1:2">
+      <c r="A825" t="s">
+        <v>6</v>
+      </c>
+      <c r="B825" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="826" spans="1:2">
+      <c r="A826" t="s">
+        <v>8</v>
+      </c>
+      <c r="B826" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="827" spans="1:2">
+      <c r="A827" t="s">
+        <v>8</v>
+      </c>
+      <c r="B827" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="828" spans="1:2">
+      <c r="A828" t="s">
+        <v>8</v>
+      </c>
+      <c r="B828" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="829" spans="1:2">
+      <c r="A829" t="s">
+        <v>8</v>
+      </c>
+      <c r="B829" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="830" spans="1:2">
+      <c r="A830" t="s">
+        <v>70</v>
+      </c>
+      <c r="B830" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="831" spans="1:2">
+      <c r="A831" t="s">
+        <v>70</v>
+      </c>
+      <c r="B831" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="832" spans="1:2">
+      <c r="A832" t="s">
+        <v>6</v>
+      </c>
+      <c r="B832" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="833" spans="1:2">
+      <c r="A833" t="s">
+        <v>6</v>
+      </c>
+      <c r="B833" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="834" spans="1:2">
+      <c r="A834" t="s">
+        <v>3</v>
+      </c>
+      <c r="B834" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="835" spans="1:2">
+      <c r="A835" t="s">
+        <v>750</v>
+      </c>
+      <c r="B835" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="836" spans="1:2">
+      <c r="A836" t="s">
+        <v>8</v>
+      </c>
+      <c r="B836" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="837" spans="1:2">
+      <c r="A837" t="s">
+        <v>8</v>
+      </c>
+      <c r="B837" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="838" spans="1:2">
+      <c r="A838" t="s">
+        <v>10</v>
+      </c>
+      <c r="B838" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="839" spans="1:2">
+      <c r="A839" t="s">
+        <v>6</v>
+      </c>
+      <c r="B839" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="840" spans="1:2">
+      <c r="A840" t="s">
+        <v>3</v>
+      </c>
+      <c r="B840" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="841" spans="1:2">
+      <c r="A841" t="s">
+        <v>6</v>
+      </c>
+      <c r="B841" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="842" spans="1:2">
+      <c r="A842" t="s">
+        <v>3</v>
+      </c>
+      <c r="B842" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="843" spans="1:2">
+      <c r="A843" t="s">
+        <v>3</v>
+      </c>
+      <c r="B843" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="844" spans="1:2">
+      <c r="A844" t="s">
+        <v>8</v>
+      </c>
+      <c r="B844" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="845" spans="1:2">
+      <c r="A845" t="s">
+        <v>3</v>
+      </c>
+      <c r="B845" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="846" spans="1:2">
+      <c r="A846" t="s">
+        <v>3</v>
+      </c>
+      <c r="B846" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="847" spans="1:2">
+      <c r="A847" t="s">
+        <v>3</v>
+      </c>
+      <c r="B847" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="848" spans="1:2">
+      <c r="A848" t="s">
+        <v>3</v>
+      </c>
+      <c r="B848" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="849" spans="1:2">
+      <c r="A849" t="s">
+        <v>748</v>
+      </c>
+      <c r="B849" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="850" spans="1:2">
+      <c r="A850" t="s">
+        <v>3</v>
+      </c>
+      <c r="B850" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="851" spans="1:2">
+      <c r="A851" t="s">
+        <v>8</v>
+      </c>
+      <c r="B851" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="852" spans="1:2">
+      <c r="A852" t="s">
+        <v>3</v>
+      </c>
+      <c r="B852" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="853" spans="1:2">
+      <c r="A853" t="s">
+        <v>10</v>
+      </c>
+      <c r="B853" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="854" spans="1:2">
+      <c r="A854" t="s">
+        <v>1</v>
+      </c>
+      <c r="B854" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="855" spans="1:2">
+      <c r="A855" t="s">
+        <v>55</v>
+      </c>
+      <c r="B855" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="856" spans="1:2">
+      <c r="A856" t="s">
+        <v>745</v>
+      </c>
+      <c r="B856" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="857" spans="1:2">
+      <c r="A857" t="s">
+        <v>1</v>
+      </c>
+      <c r="B857" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="858" spans="1:2">
+      <c r="A858" t="s">
+        <v>10</v>
+      </c>
+      <c r="B858" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="859" spans="1:2">
+      <c r="A859" t="s">
+        <v>745</v>
+      </c>
+      <c r="B859" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="860" spans="1:2">
+      <c r="A860" t="s">
+        <v>6</v>
+      </c>
+      <c r="B860" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="861" spans="1:2">
+      <c r="A861" t="s">
+        <v>6</v>
+      </c>
+      <c r="B861" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="862" spans="1:2">
+      <c r="A862" t="s">
+        <v>8</v>
+      </c>
+      <c r="B862" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="863" spans="1:2">
+      <c r="A863" t="s">
+        <v>10</v>
+      </c>
+      <c r="B863" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="864" spans="1:2">
+      <c r="A864" t="s">
+        <v>889</v>
+      </c>
+      <c r="B864" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="865" spans="1:2">
+      <c r="A865" t="s">
+        <v>3</v>
+      </c>
+      <c r="B865" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="866" spans="1:2">
+      <c r="A866" t="s">
+        <v>6</v>
+      </c>
+      <c r="B866" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="867" spans="1:2">
+      <c r="A867" t="s">
+        <v>745</v>
+      </c>
+      <c r="B867" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="868" spans="1:2">
+      <c r="A868" t="s">
+        <v>10</v>
+      </c>
+      <c r="B868" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="869" spans="1:2">
+      <c r="A869" t="s">
+        <v>183</v>
+      </c>
+      <c r="B869" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="870" spans="1:2">
+      <c r="A870" t="s">
+        <v>8</v>
+      </c>
+      <c r="B870" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="871" spans="1:2">
+      <c r="A871" t="s">
+        <v>55</v>
+      </c>
+      <c r="B871" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="872" spans="1:2">
+      <c r="A872" t="s">
+        <v>8</v>
+      </c>
+      <c r="B872" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="873" spans="1:2">
+      <c r="A873" t="s">
+        <v>3</v>
+      </c>
+      <c r="B873" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="874" spans="1:2">
+      <c r="A874" t="s">
+        <v>6</v>
+      </c>
+      <c r="B874" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="875" spans="1:2">
+      <c r="A875" t="s">
+        <v>3</v>
+      </c>
+      <c r="B875" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="876" spans="1:2">
+      <c r="A876" t="s">
+        <v>8</v>
+      </c>
+      <c r="B876" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="877" spans="1:2">
+      <c r="A877" t="s">
+        <v>750</v>
+      </c>
+      <c r="B877" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="878" spans="1:2">
+      <c r="A878" t="s">
+        <v>750</v>
+      </c>
+      <c r="B878" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="879" spans="1:2">
+      <c r="A879" t="s">
+        <v>745</v>
+      </c>
+      <c r="B879" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="880" spans="1:2">
+      <c r="A880" t="s">
+        <v>745</v>
+      </c>
+      <c r="B880" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="881" spans="1:2">
+      <c r="A881" t="s">
+        <v>3</v>
+      </c>
+      <c r="B881" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="882" spans="1:2">
+      <c r="A882" t="s">
+        <v>1</v>
+      </c>
+      <c r="B882" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="883" spans="1:2">
+      <c r="A883" t="s">
+        <v>1</v>
+      </c>
+      <c r="B883" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="884" spans="1:2">
+      <c r="A884" t="s">
+        <v>745</v>
+      </c>
+      <c r="B884" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="885" spans="1:2">
+      <c r="A885" t="s">
+        <v>70</v>
+      </c>
+      <c r="B885" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="886" spans="1:2">
+      <c r="A886" t="s">
+        <v>3</v>
+      </c>
+      <c r="B886" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="887" spans="1:2">
+      <c r="A887" t="s">
+        <v>423</v>
+      </c>
+      <c r="B887" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="888" spans="1:2">
+      <c r="A888" t="s">
+        <v>1</v>
+      </c>
+      <c r="B888" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="889" spans="1:2">
+      <c r="A889" t="s">
+        <v>915</v>
+      </c>
+      <c r="B889" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="890" spans="1:2">
+      <c r="A890" t="s">
+        <v>750</v>
+      </c>
+      <c r="B890" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="891" spans="1:2">
+      <c r="A891" t="s">
+        <v>750</v>
+      </c>
+      <c r="B891" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="892" spans="1:2">
+      <c r="A892" t="s">
+        <v>750</v>
+      </c>
+      <c r="B892" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="893" spans="1:2">
+      <c r="A893" t="s">
+        <v>750</v>
+      </c>
+      <c r="B893" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="894" spans="1:2">
+      <c r="A894" t="s">
+        <v>750</v>
+      </c>
+      <c r="B894" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="895" spans="1:2">
+      <c r="A895" t="s">
+        <v>750</v>
+      </c>
+      <c r="B895" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="896" spans="1:2">
+      <c r="A896" t="s">
+        <v>750</v>
+      </c>
+      <c r="B896" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="897" spans="1:2">
+      <c r="A897" t="s">
+        <v>10</v>
+      </c>
+      <c r="B897" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="898" spans="1:2">
+      <c r="A898" t="s">
+        <v>43</v>
+      </c>
+      <c r="B898" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="899" spans="1:2">
+      <c r="A899" t="s">
+        <v>43</v>
+      </c>
+      <c r="B899" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="900" spans="1:2">
+      <c r="A900" t="s">
+        <v>43</v>
+      </c>
+      <c r="B900" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="901" spans="1:2">
+      <c r="A901" t="s">
+        <v>43</v>
+      </c>
+      <c r="B901" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="902" spans="1:2">
+      <c r="A902" t="s">
+        <v>43</v>
+      </c>
+      <c r="B902" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="903" spans="1:2">
+      <c r="A903" t="s">
+        <v>43</v>
+      </c>
+      <c r="B903" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="904" spans="1:2">
+      <c r="A904" t="s">
+        <v>43</v>
+      </c>
+      <c r="B904" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="905" spans="1:2">
+      <c r="A905" t="s">
+        <v>43</v>
+      </c>
+      <c r="B905" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="906" spans="1:2">
+      <c r="A906" t="s">
+        <v>43</v>
+      </c>
+      <c r="B906" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="907" spans="1:2">
+      <c r="A907" t="s">
+        <v>55</v>
+      </c>
+      <c r="B907" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="908" spans="1:2">
+      <c r="A908" t="s">
+        <v>1</v>
+      </c>
+      <c r="B908" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="909" spans="1:2">
+      <c r="A909" t="s">
+        <v>70</v>
+      </c>
+      <c r="B909" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="910" spans="1:2">
+      <c r="A910" t="s">
+        <v>70</v>
+      </c>
+      <c r="B910" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="911" spans="1:2">
+      <c r="A911" t="s">
+        <v>70</v>
+      </c>
+      <c r="B911" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="912" spans="1:2">
+      <c r="A912" t="s">
+        <v>70</v>
+      </c>
+      <c r="B912" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="913" spans="1:2">
+      <c r="A913" t="s">
+        <v>70</v>
+      </c>
+      <c r="B913" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="914" spans="1:2">
+      <c r="A914" t="s">
+        <v>1</v>
+      </c>
+      <c r="B914" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="915" spans="1:2">
+      <c r="A915" t="s">
+        <v>3</v>
+      </c>
+      <c r="B915" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="916" spans="1:2">
+      <c r="A916" t="s">
+        <v>3</v>
+      </c>
+      <c r="B916" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="917" spans="1:2">
+      <c r="A917" t="s">
+        <v>3</v>
+      </c>
+      <c r="B917" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="918" spans="1:2">
+      <c r="A918" t="s">
+        <v>6</v>
+      </c>
+      <c r="B918" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="919" spans="1:2">
+      <c r="A919" t="s">
+        <v>3</v>
+      </c>
+      <c r="B919" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="920" spans="1:2">
+      <c r="A920" t="s">
+        <v>242</v>
+      </c>
+      <c r="B920" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="921" spans="1:2">
+      <c r="A921" t="s">
+        <v>3</v>
+      </c>
+      <c r="B921" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="922" spans="1:2">
+      <c r="A922" t="s">
+        <v>6</v>
+      </c>
+      <c r="B922" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="923" spans="1:2">
+      <c r="A923" t="s">
+        <v>6</v>
+      </c>
+      <c r="B923" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="924" spans="1:2">
+      <c r="A924" t="s">
+        <v>183</v>
+      </c>
+      <c r="B924" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="925" spans="1:2">
+      <c r="A925" t="s">
+        <v>6</v>
+      </c>
+      <c r="B925" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="926" spans="1:2">
+      <c r="A926" t="s">
+        <v>183</v>
+      </c>
+      <c r="B926" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="927" spans="1:2">
+      <c r="A927" t="s">
+        <v>210</v>
+      </c>
+      <c r="B927" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="928" spans="1:2">
+      <c r="A928" t="s">
+        <v>6</v>
+      </c>
+      <c r="B928" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="929" spans="1:2">
+      <c r="A929" t="s">
+        <v>3</v>
+      </c>
+      <c r="B929" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="930" spans="1:2">
+      <c r="A930" t="s">
+        <v>242</v>
+      </c>
+      <c r="B930" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="931" spans="1:2">
+      <c r="A931" t="s">
+        <v>242</v>
+      </c>
+      <c r="B931" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="932" spans="1:2">
+      <c r="A932" t="s">
+        <v>10</v>
+      </c>
+      <c r="B932" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="933" spans="1:2">
+      <c r="A933" t="s">
+        <v>10</v>
+      </c>
+      <c r="B933" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="934" spans="1:2">
+      <c r="A934" t="s">
+        <v>1</v>
+      </c>
+      <c r="B934" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="935" spans="1:2">
+      <c r="A935" t="s">
+        <v>1</v>
+      </c>
+      <c r="B935" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="936" spans="1:2">
+      <c r="A936" t="s">
+        <v>1</v>
+      </c>
+      <c r="B936" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="937" spans="1:2">
+      <c r="A937" t="s">
+        <v>1</v>
+      </c>
+      <c r="B937" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="938" spans="1:2">
+      <c r="A938" t="s">
+        <v>3</v>
+      </c>
+      <c r="B938" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="939" spans="1:2">
+      <c r="A939" t="s">
+        <v>3</v>
+      </c>
+      <c r="B939" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="940" spans="1:2">
+      <c r="A940" t="s">
+        <v>242</v>
+      </c>
+      <c r="B940" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="941" spans="1:2">
+      <c r="A941" t="s">
+        <v>3</v>
+      </c>
+      <c r="B941" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="942" spans="1:2">
+      <c r="A942" t="s">
+        <v>8</v>
+      </c>
+      <c r="B942" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="943" spans="1:2">
+      <c r="A943" t="s">
+        <v>10</v>
+      </c>
+      <c r="B943" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="944" spans="1:2">
+      <c r="A944" t="s">
+        <v>6</v>
+      </c>
+      <c r="B944" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="945" spans="1:2">
+      <c r="A945" t="s">
+        <v>745</v>
+      </c>
+      <c r="B945" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="946" spans="1:2">
+      <c r="A946" t="s">
+        <v>8</v>
+      </c>
+      <c r="B946" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="947" spans="1:2">
+      <c r="A947" t="s">
+        <v>55</v>
+      </c>
+      <c r="B947" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="948" spans="1:2">
+      <c r="A948" t="s">
+        <v>55</v>
+      </c>
+      <c r="B948" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="949" spans="1:2">
+      <c r="A949" t="s">
+        <v>1</v>
+      </c>
+      <c r="B949" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="950" spans="1:2">
+      <c r="A950" t="s">
+        <v>6</v>
+      </c>
+      <c r="B950" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="951" spans="1:2">
+      <c r="A951" t="s">
+        <v>8</v>
+      </c>
+      <c r="B951" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="952" spans="1:2">
+      <c r="A952" t="s">
+        <v>8</v>
+      </c>
+      <c r="B952" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="953" spans="1:2">
+      <c r="A953" t="s">
+        <v>10</v>
+      </c>
+      <c r="B953" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="954" spans="1:2">
+      <c r="A954" t="s">
+        <v>10</v>
+      </c>
+      <c r="B954" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="955" spans="1:2">
+      <c r="A955" t="s">
+        <v>183</v>
+      </c>
+      <c r="B955" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="956" spans="1:2">
+      <c r="A956" t="s">
+        <v>744</v>
+      </c>
+      <c r="B956" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="957" spans="1:2">
+      <c r="A957" t="s">
+        <v>3</v>
+      </c>
+      <c r="B957" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="958" spans="1:2">
+      <c r="A958" t="s">
+        <v>8</v>
+      </c>
+      <c r="B958" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="959" spans="1:2">
+      <c r="A959" t="s">
+        <v>10</v>
+      </c>
+      <c r="B959" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="960" spans="1:2">
+      <c r="A960" t="s">
+        <v>3</v>
+      </c>
+      <c r="B960" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="961" spans="1:2">
+      <c r="A961" t="s">
+        <v>8</v>
+      </c>
+      <c r="B961" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="962" spans="1:2">
+      <c r="A962" t="s">
+        <v>423</v>
+      </c>
+      <c r="B962" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="963" spans="1:2">
+      <c r="A963" t="s">
+        <v>8</v>
+      </c>
+      <c r="B963" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="964" spans="1:2">
+      <c r="A964" t="s">
+        <v>1</v>
+      </c>
+      <c r="B964" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="965" spans="1:2">
+      <c r="A965" t="s">
+        <v>55</v>
+      </c>
+      <c r="B965" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="966" spans="1:2">
+      <c r="A966" t="s">
+        <v>3</v>
+      </c>
+      <c r="B966" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="967" spans="1:2">
+      <c r="A967" t="s">
+        <v>10</v>
+      </c>
+      <c r="B967" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="968" spans="1:2">
+      <c r="A968" t="s">
+        <v>3</v>
+      </c>
+      <c r="B968" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="969" spans="1:2">
+      <c r="A969" t="s">
+        <v>8</v>
+      </c>
+      <c r="B969" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="970" spans="1:2">
+      <c r="A970" t="s">
+        <v>3</v>
+      </c>
+      <c r="B970" t="s">
+        <v>997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated categories with new data from v.123
</commit_message>
<xml_diff>
--- a/data/raw/ExtraCategoriesArchaea.xlsx
+++ b/data/raw/ExtraCategoriesArchaea.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="0" windowWidth="26160" windowHeight="17540" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="998">
   <si>
     <t>0-7.5 cm soil sample from a meadow incubated as anoxic slurry</t>
   </si>
@@ -2278,6 +2278,741 @@
   </si>
   <si>
     <t>ZN</t>
+  </si>
+  <si>
+    <t>10-20 meters below sea level off the coast of Santa Barbara, CA, USA</t>
+  </si>
+  <si>
+    <t>10% Pt methanogenic biocathode</t>
+  </si>
+  <si>
+    <t>A pilot-scale bioreactor, BRGM, France</t>
+  </si>
+  <si>
+    <t>abomasum</t>
+  </si>
+  <si>
+    <t>acid hot spring</t>
+  </si>
+  <si>
+    <t>Acid Mine Los Rueldos</t>
+  </si>
+  <si>
+    <t>acid sulfate soils</t>
+  </si>
+  <si>
+    <t>acidic paddy soil</t>
+  </si>
+  <si>
+    <t>Adriatic sea</t>
+  </si>
+  <si>
+    <t>alpine lake sediment</t>
+  </si>
+  <si>
+    <t>anaerobic bioreactor for auto-generative high pressure digestion</t>
+  </si>
+  <si>
+    <t>anaerobic, low pH pit mud of Luzhou-flavor liquor</t>
+  </si>
+  <si>
+    <t>anode biofilm in microbial fuel cells</t>
+  </si>
+  <si>
+    <t>Aran-Bidgol salt lake</t>
+  </si>
+  <si>
+    <t>Ayakekum salt lake - low temperature, low nutrient levels, abundant sunlight and remote geographical location; pH of the water was approximately pH 7-8</t>
+  </si>
+  <si>
+    <t>Ayakekumsalt Lake</t>
+  </si>
+  <si>
+    <t>Baltic Sea Thaumarchaeota enrichment culture</t>
+  </si>
+  <si>
+    <t>Banaskatha coal mine</t>
+  </si>
+  <si>
+    <t>base of Lung Snack Piccard Beebee Woods Mound Mid Cayman Rise</t>
+  </si>
+  <si>
+    <t>biofilm from subsurface sulfidic cave stream</t>
+  </si>
+  <si>
+    <t>biogas treated cow ding</t>
+  </si>
+  <si>
+    <t>bioleaching process</t>
+  </si>
+  <si>
+    <t>biomass at the Mediterranean DCM (50m)</t>
+  </si>
+  <si>
+    <t>Black Sea salt</t>
+  </si>
+  <si>
+    <t>Black smoker chimney at the Kairei field in the Central Indian Ridge</t>
+  </si>
+  <si>
+    <t>body brine (salinity 120g/L) of Thetis anoxic lake 3500m, Southern Ionian Sea</t>
+  </si>
+  <si>
+    <t>body brine (salinity 220g/L) of Thetis anoxic lake 3500m, Southern Ionian Sea</t>
+  </si>
+  <si>
+    <t>Bolivian salt</t>
+  </si>
+  <si>
+    <t>Brancoveanu lake</t>
+  </si>
+  <si>
+    <t>Brazilian Caatinga soil</t>
+  </si>
+  <si>
+    <t>Brine</t>
+  </si>
+  <si>
+    <t>brine from hypersaline Lake Medee</t>
+  </si>
+  <si>
+    <t>brine sample</t>
+  </si>
+  <si>
+    <t>brine sample from Aran-Bidgol salt lake</t>
+  </si>
+  <si>
+    <t>brine sample from salt lake</t>
+  </si>
+  <si>
+    <t>Brine-seawater interface of Atlantis II Deep, Red Sea</t>
+  </si>
+  <si>
+    <t>Brine-seawater interface of Discovery Deep, Red Sea</t>
+  </si>
+  <si>
+    <t>Brine-seawater interface of Erba Deep, Red Sea</t>
+  </si>
+  <si>
+    <t>Brine-seawater interface of Kebrit Deep, Red Sea</t>
+  </si>
+  <si>
+    <t>Brine-seawater interface of Nereus Deep, Red Sea</t>
+  </si>
+  <si>
+    <t>Camargue salt</t>
+  </si>
+  <si>
+    <t>cellulose anaerobic digester</t>
+  </si>
+  <si>
+    <t>Chardonnay salt</t>
+  </si>
+  <si>
+    <t>Cistern Spring (CIS_19); temperature 78C; pH 4.4</t>
+  </si>
+  <si>
+    <t>clay from marine sediments 136 meters below sea floor depth collected from drilling site U1352C during the IODP 317 cruise</t>
+  </si>
+  <si>
+    <t>clay from marine sediments 31 meters below sea floor depth collected from drilling site U1352C during the IODP 317 cruise</t>
+  </si>
+  <si>
+    <t>clone from PCR product of water sample</t>
+  </si>
+  <si>
+    <t>coastal surface water from the Northern Adriatic Sea</t>
+  </si>
+  <si>
+    <t>coastal/estuarine sediments</t>
+  </si>
+  <si>
+    <t>colonic digesta of grown pigs</t>
+  </si>
+  <si>
+    <t>colonic digesta of young pigs</t>
+  </si>
+  <si>
+    <t>colonic mucosa of grown pigs</t>
+  </si>
+  <si>
+    <t>column bioleaching</t>
+  </si>
+  <si>
+    <t>combined biofilm from UBA (pink subaerial biofilm) and UBA BS (thick floating biofilm subdivided into strips) samples</t>
+  </si>
+  <si>
+    <t>commercial biogas plant</t>
+  </si>
+  <si>
+    <t>constructed wetland for wastewater treatment</t>
+  </si>
+  <si>
+    <t>Copahue geotherma field, Neuquen, Argentina</t>
+  </si>
+  <si>
+    <t>Crater Hills, Alice Spring (CH-AS); temperature 75C; pH 2.5</t>
+  </si>
+  <si>
+    <t>Dabancheng salt lake</t>
+  </si>
+  <si>
+    <t>deep sea surface sediment</t>
+  </si>
+  <si>
+    <t>dental human plaque of periodontitis patients</t>
+  </si>
+  <si>
+    <t>derived from human gut metagenome</t>
+  </si>
+  <si>
+    <t>discovery brine interface of Red Sea</t>
+  </si>
+  <si>
+    <t>Drake Passage</t>
+  </si>
+  <si>
+    <t>East Pacific Ridge</t>
+  </si>
+  <si>
+    <t>Eastern Lau Spreading Center</t>
+  </si>
+  <si>
+    <t>Eel River Basin carbonate 2688</t>
+  </si>
+  <si>
+    <t>Eel River Basin sediment 2688</t>
+  </si>
+  <si>
+    <t>Eel River sediment</t>
+  </si>
+  <si>
+    <t>enrichment culture fed with acetate and methanol at 35 degrees in a sequencing batch reactor (SBR)</t>
+  </si>
+  <si>
+    <t>enrichment fermentation of pig feces with beta-glucan substrate</t>
+  </si>
+  <si>
+    <t>enrichment fermentation of pig feces without beta-glucan substrate</t>
+  </si>
+  <si>
+    <t>evaporitic salt crystal</t>
+  </si>
+  <si>
+    <t>extreme hypersaline lake water from Lake Tyrrell</t>
+  </si>
+  <si>
+    <t>extremely saline anoxic brine of the deep-sea hypersaline anoxic lake (DHAL) Thetis located South-East of the Medriff corridor collected during oceanographic cruises of the RV Urania in September 2009</t>
+  </si>
+  <si>
+    <t>Fara Fund lake</t>
+  </si>
+  <si>
+    <t>feces; sample TS28</t>
+  </si>
+  <si>
+    <t>feces; sample TS29</t>
+  </si>
+  <si>
+    <t>fermentative hydrogen production biomass</t>
+  </si>
+  <si>
+    <t>filtered surface water from Lake Tyrrell</t>
+  </si>
+  <si>
+    <t>freshwater fish tank</t>
+  </si>
+  <si>
+    <t>freshwater hot-pool in Kuirau Park</t>
+  </si>
+  <si>
+    <t>freshwater lake sediment grown in bioreactor fed with nitrate, ammonium and methane</t>
+  </si>
+  <si>
+    <t>fumarolic soil at 65 degrees C, pH8</t>
+  </si>
+  <si>
+    <t>Gangxi solar saltern, an artificial marine solar saltern</t>
+  </si>
+  <si>
+    <t>Gozo Island salt</t>
+  </si>
+  <si>
+    <t>granular sludge from a brewing industry</t>
+  </si>
+  <si>
+    <t>graphite block methanogenic biocathode</t>
+  </si>
+  <si>
+    <t>Guaymas Basin</t>
+  </si>
+  <si>
+    <t>Guaymas Basin Hydrothermal Plumes and Background; water depths 1600, 1775, 1900, 1996 m</t>
+  </si>
+  <si>
+    <t>Guerande salt</t>
+  </si>
+  <si>
+    <t>Gulf of Maine surface waters</t>
+  </si>
+  <si>
+    <t>Gulf of Mexico, Mississippi Canyon, MC118, sediments</t>
+  </si>
+  <si>
+    <t>Halen Mon salt</t>
+  </si>
+  <si>
+    <t>Halophytes</t>
+  </si>
+  <si>
+    <t>Himalayan pink salt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hot cracks </t>
+  </si>
+  <si>
+    <t>hot marine sediment</t>
+  </si>
+  <si>
+    <t>Hot spring</t>
+  </si>
+  <si>
+    <t>Hot spring in Mutnovsky Volcano</t>
+  </si>
+  <si>
+    <t>hot spring water and gravel</t>
+  </si>
+  <si>
+    <t>hot springs at Los Azufres National Park</t>
+  </si>
+  <si>
+    <t>human brain abscess</t>
+  </si>
+  <si>
+    <t>human stool specimen</t>
+  </si>
+  <si>
+    <t>Hydrate Ridge carbonate 2518</t>
+  </si>
+  <si>
+    <t>Hydrate Ridge sediment 2518</t>
+  </si>
+  <si>
+    <t>Hydrate Ridge, OR</t>
+  </si>
+  <si>
+    <t>hydrocarbon-contaminated sediment, Bemidji core 1110</t>
+  </si>
+  <si>
+    <t>hydrothermal carbonate rock</t>
+  </si>
+  <si>
+    <t>hydrothermal plume and surrounding water mass above the active hydrothermal field of the Southwest Indian Ridge</t>
+  </si>
+  <si>
+    <t>hypermesophilic terephthalate degrading bioreactor</t>
+  </si>
+  <si>
+    <t>hypersaline chloride sulfate lake of Kulunda Steppe</t>
+  </si>
+  <si>
+    <t>hypersaline endoevaporitic microbial mat</t>
+  </si>
+  <si>
+    <t>Hypersaline microbial mat</t>
+  </si>
+  <si>
+    <t>hypersaline produced water from the campos basin</t>
+  </si>
+  <si>
+    <t>hypersaline sample from solar saltern, pond crsytalizer CR30</t>
+  </si>
+  <si>
+    <t>hypersaline spring</t>
+  </si>
+  <si>
+    <t>hypersaline water sample from Lake Tyrrell</t>
+  </si>
+  <si>
+    <t>hypersaline waters of Lake Tyrrell</t>
+  </si>
+  <si>
+    <t>interface from Kryos DHAL 3337m</t>
+  </si>
+  <si>
+    <t>Ionian sea</t>
+  </si>
+  <si>
+    <t>iron corrossion-inducing microbial community</t>
+  </si>
+  <si>
+    <t>isolated as part of a large dataset composed predominantly from surface water marine samples collected along a voyage from Eastern North American coast to the Eastern Pacific Ocean, including locations in the Sargasso Sea, Panama Canal, and the Galapagos Islands</t>
+  </si>
+  <si>
+    <t>Joseph's Coat Hot Spring, Scorodite Spring (JC3A); temperature 80C; pH 6.1</t>
+  </si>
+  <si>
+    <t>La Palma Flor de Sal</t>
+  </si>
+  <si>
+    <t>lab scale mesophilic 35 C anaerobic semi-continuous digesters fed with dairy farm wastes</t>
+  </si>
+  <si>
+    <t>Lac Rose salt</t>
+  </si>
+  <si>
+    <t>Lake Tyrrell</t>
+  </si>
+  <si>
+    <t>lowermost (B1B) sediment-attached strata from acid streamer/mats thriving at Los Rueldos abandoned Hg mine</t>
+  </si>
+  <si>
+    <t>Maras salt</t>
+  </si>
+  <si>
+    <t>Marine bioreactor</t>
+  </si>
+  <si>
+    <t>marine oilfield, North sea</t>
+  </si>
+  <si>
+    <t>Marine sediment from Hiroshima Bay</t>
+  </si>
+  <si>
+    <t>marine sediment taken 10 cm below seafloor</t>
+  </si>
+  <si>
+    <t>Marker113 at caldera of Axial Seamount</t>
+  </si>
+  <si>
+    <t>mesophilic (35oC) anaerobic digesters fed by diary farm waste</t>
+  </si>
+  <si>
+    <t>BDBD</t>
+  </si>
+  <si>
+    <t>mesophilic anaerobic digester treating municipal wastewater sludge</t>
+  </si>
+  <si>
+    <t>Metagenomic fosmid libraries constructed from a methanotrophic microbial mat growing in the Black Sea</t>
+  </si>
+  <si>
+    <t>Methane hydrate sediment</t>
+  </si>
+  <si>
+    <t>mine environment soil</t>
+  </si>
+  <si>
+    <t>mixture of activated sludge and methanogenic sludge; day 435</t>
+  </si>
+  <si>
+    <t>mud of drilling swamp</t>
+  </si>
+  <si>
+    <t>mud sample collected next to a hot spring at the Los Azufres geothermal field</t>
+  </si>
+  <si>
+    <t>natural gas-associated formation water in aquifers</t>
+  </si>
+  <si>
+    <t>Norris Geyser Basin, Beowulf Spring (NGB-BED); temperature 65C; pH 3.0</t>
+  </si>
+  <si>
+    <t>Nyegga cold-seep field located at the mid-Norwegian margin on the northern edge of the Storegga Slide</t>
+  </si>
+  <si>
+    <t>Ocean drilling core sample</t>
+  </si>
+  <si>
+    <t>Ocean water at 3 m depth at station HL4 from Atlantic Zone Monitoring Program (AZMP)</t>
+  </si>
+  <si>
+    <t>Ocnei Lake</t>
+  </si>
+  <si>
+    <t>oil field water</t>
+  </si>
+  <si>
+    <t>oil formation water</t>
+  </si>
+  <si>
+    <t>Oil sands tailings enrichment culture</t>
+  </si>
+  <si>
+    <t>oil-field</t>
+  </si>
+  <si>
+    <t>oil-immersed sample from Guaymas Basin</t>
+  </si>
+  <si>
+    <t>Pakistani rock salt</t>
+  </si>
+  <si>
+    <t>Persian blue rock salt</t>
+  </si>
+  <si>
+    <t>pink biofilm microbial community collected from flowing acid mine drainage (pH 0.8, 42C)</t>
+  </si>
+  <si>
+    <t>plumage</t>
+  </si>
+  <si>
+    <t>Qi'ao Island</t>
+  </si>
+  <si>
+    <t>Qinshui basin coalbed water</t>
+  </si>
+  <si>
+    <t>raw salt</t>
+  </si>
+  <si>
+    <t>AQR</t>
+  </si>
+  <si>
+    <t>reed roots from a constructed wetland</t>
+  </si>
+  <si>
+    <t>refuse dump Nest 11 layer 3</t>
+  </si>
+  <si>
+    <t>refuse dump Nest 12 layer 0</t>
+  </si>
+  <si>
+    <t>refuse dump Nest 12 layer 1</t>
+  </si>
+  <si>
+    <t>refuse dump Nest 12 layer 2</t>
+  </si>
+  <si>
+    <t>refuse dump Nest 12 layer 4</t>
+  </si>
+  <si>
+    <t>refuse dump Nest 9 layer 0</t>
+  </si>
+  <si>
+    <t>refuse dump Nest 9 layer 2</t>
+  </si>
+  <si>
+    <t>refuse dump Nest 9 layer 4</t>
+  </si>
+  <si>
+    <t>rhizosphere of Abutilon</t>
+  </si>
+  <si>
+    <t>rhizosphere of Banni grass</t>
+  </si>
+  <si>
+    <t>rhizosphere of Cenchrus setigerus</t>
+  </si>
+  <si>
+    <t>rhizosphere of Cressa cretica</t>
+  </si>
+  <si>
+    <t>rhizosphere of Dicanthium</t>
+  </si>
+  <si>
+    <t>rhizosphere of Oain plant</t>
+  </si>
+  <si>
+    <t>rhizosphere of plant of Asteraceae family</t>
+  </si>
+  <si>
+    <t>rhizosphere of Sporobolus</t>
+  </si>
+  <si>
+    <t>rhizosphere of Suaeda nudiflora</t>
+  </si>
+  <si>
+    <t>Rifle groundwater metagenome at time 1 / A; 0.2 micron filter</t>
+  </si>
+  <si>
+    <t>rock salt drill core samples from the depth of ~800 m, Yunying salt mine</t>
+  </si>
+  <si>
+    <t>rumen fluid of Dechang buffalo</t>
+  </si>
+  <si>
+    <t>rumen fluid of Dechang buffalorumen fluid of Dechang buffalorumen fluid of Dechang buffalo</t>
+  </si>
+  <si>
+    <t>rumen fluid of water buffalo</t>
+  </si>
+  <si>
+    <t>rumen fluid of water buffalo in China</t>
+  </si>
+  <si>
+    <t>rumen methanogens from Budorcas taxicolor bedfordi</t>
+  </si>
+  <si>
+    <t>saline soil from Tarim Basin</t>
+  </si>
+  <si>
+    <t>salt crystallizer Little Rann of Kutch</t>
+  </si>
+  <si>
+    <t>Salt Crystallizer Pond</t>
+  </si>
+  <si>
+    <t>salt crystallizer pond</t>
+  </si>
+  <si>
+    <t>salt lake sediments</t>
+  </si>
+  <si>
+    <t>saltern pond</t>
+  </si>
+  <si>
+    <t>Saltern solar multipond</t>
+  </si>
+  <si>
+    <t>seawater filtered on 0.2 um membrane filter at a depth of 60m, temperature: 13.53 celsius degree, salinity: 34.85, dissolved oxygen concentration:1.8 uM</t>
+  </si>
+  <si>
+    <t>sediment associated with methane hydrate from Krishna Godavari Basin</t>
+  </si>
+  <si>
+    <t>sediment from saline lake</t>
+  </si>
+  <si>
+    <t>sediment of pond</t>
+  </si>
+  <si>
+    <t>sediment of reec</t>
+  </si>
+  <si>
+    <t>sediment of reed</t>
+  </si>
+  <si>
+    <t>sediment-brine interface of the Shaban Deep in the Red Sea</t>
+  </si>
+  <si>
+    <t>sediments from an inland lake</t>
+  </si>
+  <si>
+    <t>Sheyang marine solar saltern</t>
+  </si>
+  <si>
+    <t>single cell amplified by MDA; Atlantis II deep Red Sea brine-seawater interface</t>
+  </si>
+  <si>
+    <t>single cell amplified by MDA; Atlantis II Deep Red Sea brine-seawater interface</t>
+  </si>
+  <si>
+    <t>sludge from full-scale UASB reactor treating PTA wastewater</t>
+  </si>
+  <si>
+    <t>sludge layer in laboratory-scale septic tanks</t>
+  </si>
+  <si>
+    <t>soil aquifer system</t>
+  </si>
+  <si>
+    <t>soil from saline lake</t>
+  </si>
+  <si>
+    <t>soil sample from Sambhar lake</t>
+  </si>
+  <si>
+    <t>Solar salt</t>
+  </si>
+  <si>
+    <t>solar saltern at 12% salinity</t>
+  </si>
+  <si>
+    <t>solar saltern from Mohei salt mine</t>
+  </si>
+  <si>
+    <t>solar saltern water</t>
+  </si>
+  <si>
+    <t>South Atlantic</t>
+  </si>
+  <si>
+    <t>spring saltern</t>
+  </si>
+  <si>
+    <t>sub-cultured for isolation from anaerobic microbial enrichment culture derived from a coal seam gas formation water sample</t>
+  </si>
+  <si>
+    <t>submarine canyon sediments off the coast of southern California</t>
+  </si>
+  <si>
+    <t>submerged non-stratified mat biofilm (B2A) from acid streamer/mats thriving at Los Rueldos abandoned Hg mine</t>
+  </si>
+  <si>
+    <t>sulfide rock in a flange from Godzilla, an active hydrothermal vent sulfide chimney in the High Rise Hydrothermal vent field (at 47 58.00'N and 129 05.50'W), along the Endeavour segment of the Juan de Fuca Ridge, at a depth of 2144 m, approximately 300 miles west of Seattle, in the Northeast Pacific Ocean</t>
+  </si>
+  <si>
+    <t>sulfidic aquifer Muehlbacher Schwefelquelle</t>
+  </si>
+  <si>
+    <t>sulfidic groundwater</t>
+  </si>
+  <si>
+    <t>sulfur and silica sinter at air/water interface</t>
+  </si>
+  <si>
+    <t>surficial sediments beneath a 12-ft water column from coastal/estuarine sediments</t>
+  </si>
+  <si>
+    <t>thermal and acidic green biofilms from a fumarole</t>
+  </si>
+  <si>
+    <t>thermal soil</t>
+  </si>
+  <si>
+    <t>thermophilic electromethanogenic bioelectrochemical reactor biocathode</t>
+  </si>
+  <si>
+    <t>thermophilic sludge anaerobic digestion</t>
+  </si>
+  <si>
+    <t>total DNA isolated from fresh water sediment, Nov. 2003, Orsay, France</t>
+  </si>
+  <si>
+    <t>Traditional salt-fermented seafood in Korea</t>
+  </si>
+  <si>
+    <t>transitional zone</t>
+  </si>
+  <si>
+    <t>two 30-60 cm subsurface water samples (65C) from the hot springs at Los Azufres National Park</t>
+  </si>
+  <si>
+    <t>UAFB system treated with terephthalate contained wastewater</t>
+  </si>
+  <si>
+    <t>Upper convective layer of Atlantis II Deep, Red Sea</t>
+  </si>
+  <si>
+    <t>walls of a black smoker at a deep-sea hydrothermal vent, 9</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>water from hydrothermal chimney-like structure</t>
+  </si>
+  <si>
+    <t>White Rann soil</t>
+  </si>
+  <si>
+    <t>White Rann water</t>
+  </si>
+  <si>
+    <t>Yangjiang marine solar saltern</t>
+  </si>
+  <si>
+    <t>yellow water of Chinese intense flavor liquor cellar</t>
+  </si>
+  <si>
+    <t>Yinggehai marine solar saltern</t>
+  </si>
+  <si>
+    <t>Zara Saltern, Sivas (spring saltern)</t>
+  </si>
+  <si>
+    <t>Zhoushan marine solar saltern</t>
   </si>
 </sst>
 </file>
@@ -2858,15 +3593,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B727"/>
+  <dimension ref="A1:B970"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A420" workbookViewId="0">
+      <selection activeCell="B440" sqref="B440"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="122.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8684,6 +9419,1950 @@
       </c>
       <c r="B727" t="s">
         <v>743</v>
+      </c>
+    </row>
+    <row r="728" spans="1:2">
+      <c r="A728" t="s">
+        <v>3</v>
+      </c>
+      <c r="B728" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="729" spans="1:2">
+      <c r="A729" t="s">
+        <v>10</v>
+      </c>
+      <c r="B729" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="730" spans="1:2">
+      <c r="A730" t="s">
+        <v>10</v>
+      </c>
+      <c r="B730" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="731" spans="1:2">
+      <c r="A731" t="s">
+        <v>70</v>
+      </c>
+      <c r="B731" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="732" spans="1:2">
+      <c r="A732" t="s">
+        <v>8</v>
+      </c>
+      <c r="B732" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="733" spans="1:2">
+      <c r="A733" t="s">
+        <v>745</v>
+      </c>
+      <c r="B733" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="734" spans="1:2">
+      <c r="A734" t="s">
+        <v>1</v>
+      </c>
+      <c r="B734" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="735" spans="1:2">
+      <c r="A735" t="s">
+        <v>1</v>
+      </c>
+      <c r="B735" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="736" spans="1:2">
+      <c r="A736" t="s">
+        <v>3</v>
+      </c>
+      <c r="B736" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="737" spans="1:2">
+      <c r="A737" t="s">
+        <v>183</v>
+      </c>
+      <c r="B737" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="738" spans="1:2">
+      <c r="A738" t="s">
+        <v>10</v>
+      </c>
+      <c r="B738" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="739" spans="1:2">
+      <c r="A739" t="s">
+        <v>183</v>
+      </c>
+      <c r="B739" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="740" spans="1:2">
+      <c r="A740" t="s">
+        <v>10</v>
+      </c>
+      <c r="B740" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="741" spans="1:2">
+      <c r="A741" t="s">
+        <v>3</v>
+      </c>
+      <c r="B741" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="742" spans="1:2">
+      <c r="A742" t="s">
+        <v>3</v>
+      </c>
+      <c r="B742" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="743" spans="1:2">
+      <c r="A743" t="s">
+        <v>3</v>
+      </c>
+      <c r="B743" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="744" spans="1:2">
+      <c r="A744" t="s">
+        <v>3</v>
+      </c>
+      <c r="B744" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="745" spans="1:2">
+      <c r="A745" t="s">
+        <v>745</v>
+      </c>
+      <c r="B745" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="746" spans="1:2">
+      <c r="A746" t="s">
+        <v>8</v>
+      </c>
+      <c r="B746" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="747" spans="1:2">
+      <c r="A747" t="s">
+        <v>1</v>
+      </c>
+      <c r="B747" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="748" spans="1:2">
+      <c r="A748" t="s">
+        <v>10</v>
+      </c>
+      <c r="B748" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="749" spans="1:2">
+      <c r="A749" t="s">
+        <v>10</v>
+      </c>
+      <c r="B749" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="750" spans="1:2">
+      <c r="A750" t="s">
+        <v>3</v>
+      </c>
+      <c r="B750" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="751" spans="1:2">
+      <c r="A751" t="s">
+        <v>1</v>
+      </c>
+      <c r="B751" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="752" spans="1:2">
+      <c r="A752" t="s">
+        <v>8</v>
+      </c>
+      <c r="B752" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="753" spans="1:2">
+      <c r="A753" t="s">
+        <v>242</v>
+      </c>
+      <c r="B753" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="754" spans="1:2">
+      <c r="A754" t="s">
+        <v>242</v>
+      </c>
+      <c r="B754" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="755" spans="1:2">
+      <c r="A755" t="s">
+        <v>1</v>
+      </c>
+      <c r="B755" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="756" spans="1:2">
+      <c r="A756" t="s">
+        <v>55</v>
+      </c>
+      <c r="B756" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="757" spans="1:2">
+      <c r="A757" t="s">
+        <v>1</v>
+      </c>
+      <c r="B757" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="758" spans="1:2">
+      <c r="A758" t="s">
+        <v>242</v>
+      </c>
+      <c r="B758" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="759" spans="1:2">
+      <c r="A759" t="s">
+        <v>242</v>
+      </c>
+      <c r="B759" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="760" spans="1:2">
+      <c r="A760" t="s">
+        <v>242</v>
+      </c>
+      <c r="B760" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="761" spans="1:2">
+      <c r="A761" t="s">
+        <v>242</v>
+      </c>
+      <c r="B761" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="762" spans="1:2">
+      <c r="A762" t="s">
+        <v>242</v>
+      </c>
+      <c r="B762" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="763" spans="1:2">
+      <c r="A763" t="s">
+        <v>242</v>
+      </c>
+      <c r="B763" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="764" spans="1:2">
+      <c r="A764" t="s">
+        <v>242</v>
+      </c>
+      <c r="B764" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="765" spans="1:2">
+      <c r="A765" t="s">
+        <v>242</v>
+      </c>
+      <c r="B765" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="766" spans="1:2">
+      <c r="A766" t="s">
+        <v>242</v>
+      </c>
+      <c r="B766" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="767" spans="1:2">
+      <c r="A767" t="s">
+        <v>242</v>
+      </c>
+      <c r="B767" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="768" spans="1:2">
+      <c r="A768" t="s">
+        <v>1</v>
+      </c>
+      <c r="B768" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="769" spans="1:2">
+      <c r="A769" t="s">
+        <v>10</v>
+      </c>
+      <c r="B769" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="770" spans="1:2">
+      <c r="A770" t="s">
+        <v>1</v>
+      </c>
+      <c r="B770" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="771" spans="1:2">
+      <c r="A771" t="s">
+        <v>8</v>
+      </c>
+      <c r="B771" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="772" spans="1:2">
+      <c r="A772" t="s">
+        <v>6</v>
+      </c>
+      <c r="B772" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="773" spans="1:2">
+      <c r="A773" t="s">
+        <v>6</v>
+      </c>
+      <c r="B773" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="774" spans="1:2">
+      <c r="A774" t="s">
+        <v>423</v>
+      </c>
+      <c r="B774" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="775" spans="1:2">
+      <c r="A775" t="s">
+        <v>3</v>
+      </c>
+      <c r="B775" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="776" spans="1:2">
+      <c r="A776" t="s">
+        <v>210</v>
+      </c>
+      <c r="B776" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="777" spans="1:2">
+      <c r="A777" t="s">
+        <v>70</v>
+      </c>
+      <c r="B777" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="778" spans="1:2">
+      <c r="A778" t="s">
+        <v>70</v>
+      </c>
+      <c r="B778" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="779" spans="1:2">
+      <c r="A779" t="s">
+        <v>70</v>
+      </c>
+      <c r="B779" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="780" spans="1:2">
+      <c r="A780" t="s">
+        <v>745</v>
+      </c>
+      <c r="B780" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="781" spans="1:2">
+      <c r="A781" t="s">
+        <v>10</v>
+      </c>
+      <c r="B781" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="782" spans="1:2">
+      <c r="A782" t="s">
+        <v>10</v>
+      </c>
+      <c r="B782" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="783" spans="1:2">
+      <c r="A783" t="s">
+        <v>10</v>
+      </c>
+      <c r="B783" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="784" spans="1:2">
+      <c r="A784" t="s">
+        <v>8</v>
+      </c>
+      <c r="B784" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="785" spans="1:2">
+      <c r="A785" t="s">
+        <v>8</v>
+      </c>
+      <c r="B785" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="786" spans="1:2">
+      <c r="A786" t="s">
+        <v>3</v>
+      </c>
+      <c r="B786" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="787" spans="1:2">
+      <c r="A787" t="s">
+        <v>6</v>
+      </c>
+      <c r="B787" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="788" spans="1:2">
+      <c r="A788" t="s">
+        <v>70</v>
+      </c>
+      <c r="B788" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="789" spans="1:2">
+      <c r="A789" t="s">
+        <v>70</v>
+      </c>
+      <c r="B789" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="790" spans="1:2">
+      <c r="A790" t="s">
+        <v>242</v>
+      </c>
+      <c r="B790" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="791" spans="1:2">
+      <c r="A791" t="s">
+        <v>3</v>
+      </c>
+      <c r="B791" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="792" spans="1:2">
+      <c r="A792" t="s">
+        <v>6</v>
+      </c>
+      <c r="B792" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="793" spans="1:2">
+      <c r="A793" t="s">
+        <v>6</v>
+      </c>
+      <c r="B793" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="794" spans="1:2">
+      <c r="A794" t="s">
+        <v>183</v>
+      </c>
+      <c r="B794" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="795" spans="1:2">
+      <c r="A795" t="s">
+        <v>183</v>
+      </c>
+      <c r="B795" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="796" spans="1:2">
+      <c r="A796" t="s">
+        <v>183</v>
+      </c>
+      <c r="B796" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="797" spans="1:2">
+      <c r="A797" t="s">
+        <v>10</v>
+      </c>
+      <c r="B797" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="798" spans="1:2">
+      <c r="A798" t="s">
+        <v>10</v>
+      </c>
+      <c r="B798" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="799" spans="1:2">
+      <c r="A799" t="s">
+        <v>70</v>
+      </c>
+      <c r="B799" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="800" spans="1:2">
+      <c r="A800" t="s">
+        <v>1</v>
+      </c>
+      <c r="B800" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="801" spans="1:2">
+      <c r="A801" t="s">
+        <v>3</v>
+      </c>
+      <c r="B801" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="802" spans="1:2">
+      <c r="A802" t="s">
+        <v>242</v>
+      </c>
+      <c r="B802" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="803" spans="1:2">
+      <c r="A803" t="s">
+        <v>55</v>
+      </c>
+      <c r="B803" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="804" spans="1:2">
+      <c r="A804" t="s">
+        <v>70</v>
+      </c>
+      <c r="B804" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="805" spans="1:2">
+      <c r="A805" t="s">
+        <v>70</v>
+      </c>
+      <c r="B805" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="806" spans="1:2">
+      <c r="A806" t="s">
+        <v>10</v>
+      </c>
+      <c r="B806" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="807" spans="1:2">
+      <c r="A807" t="s">
+        <v>55</v>
+      </c>
+      <c r="B807" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="808" spans="1:2">
+      <c r="A808" t="s">
+        <v>423</v>
+      </c>
+      <c r="B808" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="809" spans="1:2">
+      <c r="A809" t="s">
+        <v>8</v>
+      </c>
+      <c r="B809" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="810" spans="1:2">
+      <c r="A810" t="s">
+        <v>10</v>
+      </c>
+      <c r="B810" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="811" spans="1:2">
+      <c r="A811" t="s">
+        <v>1</v>
+      </c>
+      <c r="B811" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="812" spans="1:2">
+      <c r="A812" t="s">
+        <v>3</v>
+      </c>
+      <c r="B812" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="813" spans="1:2">
+      <c r="A813" t="s">
+        <v>1</v>
+      </c>
+      <c r="B813" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="814" spans="1:2">
+      <c r="A814" t="s">
+        <v>10</v>
+      </c>
+      <c r="B814" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="815" spans="1:2">
+      <c r="A815" t="s">
+        <v>10</v>
+      </c>
+      <c r="B815" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="816" spans="1:2">
+      <c r="A816" t="s">
+        <v>6</v>
+      </c>
+      <c r="B816" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="817" spans="1:2">
+      <c r="A817" t="s">
+        <v>8</v>
+      </c>
+      <c r="B817" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="818" spans="1:2">
+      <c r="A818" t="s">
+        <v>1</v>
+      </c>
+      <c r="B818" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="819" spans="1:2">
+      <c r="A819" t="s">
+        <v>3</v>
+      </c>
+      <c r="B819" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="820" spans="1:2">
+      <c r="A820" t="s">
+        <v>6</v>
+      </c>
+      <c r="B820" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="821" spans="1:2">
+      <c r="A821" t="s">
+        <v>1</v>
+      </c>
+      <c r="B821" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="822" spans="1:2">
+      <c r="A822" t="s">
+        <v>3</v>
+      </c>
+      <c r="B822" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="823" spans="1:2">
+      <c r="A823" t="s">
+        <v>1</v>
+      </c>
+      <c r="B823" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="824" spans="1:2">
+      <c r="A824" t="s">
+        <v>8</v>
+      </c>
+      <c r="B824" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="825" spans="1:2">
+      <c r="A825" t="s">
+        <v>6</v>
+      </c>
+      <c r="B825" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="826" spans="1:2">
+      <c r="A826" t="s">
+        <v>8</v>
+      </c>
+      <c r="B826" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="827" spans="1:2">
+      <c r="A827" t="s">
+        <v>8</v>
+      </c>
+      <c r="B827" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="828" spans="1:2">
+      <c r="A828" t="s">
+        <v>8</v>
+      </c>
+      <c r="B828" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="829" spans="1:2">
+      <c r="A829" t="s">
+        <v>8</v>
+      </c>
+      <c r="B829" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="830" spans="1:2">
+      <c r="A830" t="s">
+        <v>70</v>
+      </c>
+      <c r="B830" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="831" spans="1:2">
+      <c r="A831" t="s">
+        <v>70</v>
+      </c>
+      <c r="B831" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="832" spans="1:2">
+      <c r="A832" t="s">
+        <v>6</v>
+      </c>
+      <c r="B832" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="833" spans="1:2">
+      <c r="A833" t="s">
+        <v>6</v>
+      </c>
+      <c r="B833" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="834" spans="1:2">
+      <c r="A834" t="s">
+        <v>3</v>
+      </c>
+      <c r="B834" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="835" spans="1:2">
+      <c r="A835" t="s">
+        <v>750</v>
+      </c>
+      <c r="B835" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="836" spans="1:2">
+      <c r="A836" t="s">
+        <v>8</v>
+      </c>
+      <c r="B836" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="837" spans="1:2">
+      <c r="A837" t="s">
+        <v>8</v>
+      </c>
+      <c r="B837" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="838" spans="1:2">
+      <c r="A838" t="s">
+        <v>10</v>
+      </c>
+      <c r="B838" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="839" spans="1:2">
+      <c r="A839" t="s">
+        <v>6</v>
+      </c>
+      <c r="B839" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="840" spans="1:2">
+      <c r="A840" t="s">
+        <v>3</v>
+      </c>
+      <c r="B840" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="841" spans="1:2">
+      <c r="A841" t="s">
+        <v>6</v>
+      </c>
+      <c r="B841" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="842" spans="1:2">
+      <c r="A842" t="s">
+        <v>3</v>
+      </c>
+      <c r="B842" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="843" spans="1:2">
+      <c r="A843" t="s">
+        <v>3</v>
+      </c>
+      <c r="B843" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="844" spans="1:2">
+      <c r="A844" t="s">
+        <v>8</v>
+      </c>
+      <c r="B844" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="845" spans="1:2">
+      <c r="A845" t="s">
+        <v>3</v>
+      </c>
+      <c r="B845" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="846" spans="1:2">
+      <c r="A846" t="s">
+        <v>3</v>
+      </c>
+      <c r="B846" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="847" spans="1:2">
+      <c r="A847" t="s">
+        <v>3</v>
+      </c>
+      <c r="B847" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="848" spans="1:2">
+      <c r="A848" t="s">
+        <v>3</v>
+      </c>
+      <c r="B848" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="849" spans="1:2">
+      <c r="A849" t="s">
+        <v>748</v>
+      </c>
+      <c r="B849" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="850" spans="1:2">
+      <c r="A850" t="s">
+        <v>3</v>
+      </c>
+      <c r="B850" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="851" spans="1:2">
+      <c r="A851" t="s">
+        <v>8</v>
+      </c>
+      <c r="B851" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="852" spans="1:2">
+      <c r="A852" t="s">
+        <v>3</v>
+      </c>
+      <c r="B852" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="853" spans="1:2">
+      <c r="A853" t="s">
+        <v>10</v>
+      </c>
+      <c r="B853" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="854" spans="1:2">
+      <c r="A854" t="s">
+        <v>1</v>
+      </c>
+      <c r="B854" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="855" spans="1:2">
+      <c r="A855" t="s">
+        <v>55</v>
+      </c>
+      <c r="B855" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="856" spans="1:2">
+      <c r="A856" t="s">
+        <v>745</v>
+      </c>
+      <c r="B856" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="857" spans="1:2">
+      <c r="A857" t="s">
+        <v>1</v>
+      </c>
+      <c r="B857" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="858" spans="1:2">
+      <c r="A858" t="s">
+        <v>10</v>
+      </c>
+      <c r="B858" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="859" spans="1:2">
+      <c r="A859" t="s">
+        <v>745</v>
+      </c>
+      <c r="B859" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="860" spans="1:2">
+      <c r="A860" t="s">
+        <v>6</v>
+      </c>
+      <c r="B860" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="861" spans="1:2">
+      <c r="A861" t="s">
+        <v>6</v>
+      </c>
+      <c r="B861" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="862" spans="1:2">
+      <c r="A862" t="s">
+        <v>8</v>
+      </c>
+      <c r="B862" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="863" spans="1:2">
+      <c r="A863" t="s">
+        <v>10</v>
+      </c>
+      <c r="B863" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="864" spans="1:2">
+      <c r="A864" t="s">
+        <v>889</v>
+      </c>
+      <c r="B864" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="865" spans="1:2">
+      <c r="A865" t="s">
+        <v>3</v>
+      </c>
+      <c r="B865" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="866" spans="1:2">
+      <c r="A866" t="s">
+        <v>6</v>
+      </c>
+      <c r="B866" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="867" spans="1:2">
+      <c r="A867" t="s">
+        <v>745</v>
+      </c>
+      <c r="B867" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="868" spans="1:2">
+      <c r="A868" t="s">
+        <v>10</v>
+      </c>
+      <c r="B868" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="869" spans="1:2">
+      <c r="A869" t="s">
+        <v>183</v>
+      </c>
+      <c r="B869" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="870" spans="1:2">
+      <c r="A870" t="s">
+        <v>8</v>
+      </c>
+      <c r="B870" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="871" spans="1:2">
+      <c r="A871" t="s">
+        <v>55</v>
+      </c>
+      <c r="B871" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="872" spans="1:2">
+      <c r="A872" t="s">
+        <v>8</v>
+      </c>
+      <c r="B872" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="873" spans="1:2">
+      <c r="A873" t="s">
+        <v>3</v>
+      </c>
+      <c r="B873" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="874" spans="1:2">
+      <c r="A874" t="s">
+        <v>6</v>
+      </c>
+      <c r="B874" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="875" spans="1:2">
+      <c r="A875" t="s">
+        <v>3</v>
+      </c>
+      <c r="B875" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="876" spans="1:2">
+      <c r="A876" t="s">
+        <v>8</v>
+      </c>
+      <c r="B876" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="877" spans="1:2">
+      <c r="A877" t="s">
+        <v>750</v>
+      </c>
+      <c r="B877" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="878" spans="1:2">
+      <c r="A878" t="s">
+        <v>750</v>
+      </c>
+      <c r="B878" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="879" spans="1:2">
+      <c r="A879" t="s">
+        <v>745</v>
+      </c>
+      <c r="B879" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="880" spans="1:2">
+      <c r="A880" t="s">
+        <v>745</v>
+      </c>
+      <c r="B880" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="881" spans="1:2">
+      <c r="A881" t="s">
+        <v>3</v>
+      </c>
+      <c r="B881" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="882" spans="1:2">
+      <c r="A882" t="s">
+        <v>1</v>
+      </c>
+      <c r="B882" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="883" spans="1:2">
+      <c r="A883" t="s">
+        <v>1</v>
+      </c>
+      <c r="B883" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="884" spans="1:2">
+      <c r="A884" t="s">
+        <v>745</v>
+      </c>
+      <c r="B884" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="885" spans="1:2">
+      <c r="A885" t="s">
+        <v>70</v>
+      </c>
+      <c r="B885" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="886" spans="1:2">
+      <c r="A886" t="s">
+        <v>3</v>
+      </c>
+      <c r="B886" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="887" spans="1:2">
+      <c r="A887" t="s">
+        <v>423</v>
+      </c>
+      <c r="B887" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="888" spans="1:2">
+      <c r="A888" t="s">
+        <v>1</v>
+      </c>
+      <c r="B888" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="889" spans="1:2">
+      <c r="A889" t="s">
+        <v>915</v>
+      </c>
+      <c r="B889" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="890" spans="1:2">
+      <c r="A890" t="s">
+        <v>750</v>
+      </c>
+      <c r="B890" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="891" spans="1:2">
+      <c r="A891" t="s">
+        <v>750</v>
+      </c>
+      <c r="B891" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="892" spans="1:2">
+      <c r="A892" t="s">
+        <v>750</v>
+      </c>
+      <c r="B892" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="893" spans="1:2">
+      <c r="A893" t="s">
+        <v>750</v>
+      </c>
+      <c r="B893" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="894" spans="1:2">
+      <c r="A894" t="s">
+        <v>750</v>
+      </c>
+      <c r="B894" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="895" spans="1:2">
+      <c r="A895" t="s">
+        <v>750</v>
+      </c>
+      <c r="B895" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="896" spans="1:2">
+      <c r="A896" t="s">
+        <v>750</v>
+      </c>
+      <c r="B896" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="897" spans="1:2">
+      <c r="A897" t="s">
+        <v>10</v>
+      </c>
+      <c r="B897" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="898" spans="1:2">
+      <c r="A898" t="s">
+        <v>43</v>
+      </c>
+      <c r="B898" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="899" spans="1:2">
+      <c r="A899" t="s">
+        <v>43</v>
+      </c>
+      <c r="B899" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="900" spans="1:2">
+      <c r="A900" t="s">
+        <v>43</v>
+      </c>
+      <c r="B900" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="901" spans="1:2">
+      <c r="A901" t="s">
+        <v>43</v>
+      </c>
+      <c r="B901" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="902" spans="1:2">
+      <c r="A902" t="s">
+        <v>43</v>
+      </c>
+      <c r="B902" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="903" spans="1:2">
+      <c r="A903" t="s">
+        <v>43</v>
+      </c>
+      <c r="B903" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="904" spans="1:2">
+      <c r="A904" t="s">
+        <v>43</v>
+      </c>
+      <c r="B904" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="905" spans="1:2">
+      <c r="A905" t="s">
+        <v>43</v>
+      </c>
+      <c r="B905" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="906" spans="1:2">
+      <c r="A906" t="s">
+        <v>43</v>
+      </c>
+      <c r="B906" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="907" spans="1:2">
+      <c r="A907" t="s">
+        <v>55</v>
+      </c>
+      <c r="B907" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="908" spans="1:2">
+      <c r="A908" t="s">
+        <v>1</v>
+      </c>
+      <c r="B908" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="909" spans="1:2">
+      <c r="A909" t="s">
+        <v>70</v>
+      </c>
+      <c r="B909" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="910" spans="1:2">
+      <c r="A910" t="s">
+        <v>70</v>
+      </c>
+      <c r="B910" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="911" spans="1:2">
+      <c r="A911" t="s">
+        <v>70</v>
+      </c>
+      <c r="B911" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="912" spans="1:2">
+      <c r="A912" t="s">
+        <v>70</v>
+      </c>
+      <c r="B912" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="913" spans="1:2">
+      <c r="A913" t="s">
+        <v>70</v>
+      </c>
+      <c r="B913" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="914" spans="1:2">
+      <c r="A914" t="s">
+        <v>1</v>
+      </c>
+      <c r="B914" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="915" spans="1:2">
+      <c r="A915" t="s">
+        <v>3</v>
+      </c>
+      <c r="B915" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="916" spans="1:2">
+      <c r="A916" t="s">
+        <v>3</v>
+      </c>
+      <c r="B916" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="917" spans="1:2">
+      <c r="A917" t="s">
+        <v>3</v>
+      </c>
+      <c r="B917" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="918" spans="1:2">
+      <c r="A918" t="s">
+        <v>6</v>
+      </c>
+      <c r="B918" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="919" spans="1:2">
+      <c r="A919" t="s">
+        <v>3</v>
+      </c>
+      <c r="B919" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="920" spans="1:2">
+      <c r="A920" t="s">
+        <v>242</v>
+      </c>
+      <c r="B920" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="921" spans="1:2">
+      <c r="A921" t="s">
+        <v>3</v>
+      </c>
+      <c r="B921" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="922" spans="1:2">
+      <c r="A922" t="s">
+        <v>6</v>
+      </c>
+      <c r="B922" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="923" spans="1:2">
+      <c r="A923" t="s">
+        <v>6</v>
+      </c>
+      <c r="B923" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="924" spans="1:2">
+      <c r="A924" t="s">
+        <v>183</v>
+      </c>
+      <c r="B924" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="925" spans="1:2">
+      <c r="A925" t="s">
+        <v>6</v>
+      </c>
+      <c r="B925" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="926" spans="1:2">
+      <c r="A926" t="s">
+        <v>183</v>
+      </c>
+      <c r="B926" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="927" spans="1:2">
+      <c r="A927" t="s">
+        <v>210</v>
+      </c>
+      <c r="B927" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="928" spans="1:2">
+      <c r="A928" t="s">
+        <v>6</v>
+      </c>
+      <c r="B928" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="929" spans="1:2">
+      <c r="A929" t="s">
+        <v>3</v>
+      </c>
+      <c r="B929" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="930" spans="1:2">
+      <c r="A930" t="s">
+        <v>242</v>
+      </c>
+      <c r="B930" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="931" spans="1:2">
+      <c r="A931" t="s">
+        <v>242</v>
+      </c>
+      <c r="B931" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="932" spans="1:2">
+      <c r="A932" t="s">
+        <v>10</v>
+      </c>
+      <c r="B932" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="933" spans="1:2">
+      <c r="A933" t="s">
+        <v>10</v>
+      </c>
+      <c r="B933" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="934" spans="1:2">
+      <c r="A934" t="s">
+        <v>1</v>
+      </c>
+      <c r="B934" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="935" spans="1:2">
+      <c r="A935" t="s">
+        <v>1</v>
+      </c>
+      <c r="B935" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="936" spans="1:2">
+      <c r="A936" t="s">
+        <v>1</v>
+      </c>
+      <c r="B936" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="937" spans="1:2">
+      <c r="A937" t="s">
+        <v>1</v>
+      </c>
+      <c r="B937" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="938" spans="1:2">
+      <c r="A938" t="s">
+        <v>3</v>
+      </c>
+      <c r="B938" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="939" spans="1:2">
+      <c r="A939" t="s">
+        <v>3</v>
+      </c>
+      <c r="B939" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="940" spans="1:2">
+      <c r="A940" t="s">
+        <v>242</v>
+      </c>
+      <c r="B940" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="941" spans="1:2">
+      <c r="A941" t="s">
+        <v>3</v>
+      </c>
+      <c r="B941" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="942" spans="1:2">
+      <c r="A942" t="s">
+        <v>8</v>
+      </c>
+      <c r="B942" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="943" spans="1:2">
+      <c r="A943" t="s">
+        <v>10</v>
+      </c>
+      <c r="B943" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="944" spans="1:2">
+      <c r="A944" t="s">
+        <v>6</v>
+      </c>
+      <c r="B944" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="945" spans="1:2">
+      <c r="A945" t="s">
+        <v>745</v>
+      </c>
+      <c r="B945" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="946" spans="1:2">
+      <c r="A946" t="s">
+        <v>8</v>
+      </c>
+      <c r="B946" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="947" spans="1:2">
+      <c r="A947" t="s">
+        <v>55</v>
+      </c>
+      <c r="B947" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="948" spans="1:2">
+      <c r="A948" t="s">
+        <v>55</v>
+      </c>
+      <c r="B948" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="949" spans="1:2">
+      <c r="A949" t="s">
+        <v>1</v>
+      </c>
+      <c r="B949" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="950" spans="1:2">
+      <c r="A950" t="s">
+        <v>6</v>
+      </c>
+      <c r="B950" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="951" spans="1:2">
+      <c r="A951" t="s">
+        <v>8</v>
+      </c>
+      <c r="B951" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="952" spans="1:2">
+      <c r="A952" t="s">
+        <v>8</v>
+      </c>
+      <c r="B952" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="953" spans="1:2">
+      <c r="A953" t="s">
+        <v>10</v>
+      </c>
+      <c r="B953" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="954" spans="1:2">
+      <c r="A954" t="s">
+        <v>10</v>
+      </c>
+      <c r="B954" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="955" spans="1:2">
+      <c r="A955" t="s">
+        <v>183</v>
+      </c>
+      <c r="B955" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="956" spans="1:2">
+      <c r="A956" t="s">
+        <v>744</v>
+      </c>
+      <c r="B956" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="957" spans="1:2">
+      <c r="A957" t="s">
+        <v>3</v>
+      </c>
+      <c r="B957" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="958" spans="1:2">
+      <c r="A958" t="s">
+        <v>8</v>
+      </c>
+      <c r="B958" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="959" spans="1:2">
+      <c r="A959" t="s">
+        <v>10</v>
+      </c>
+      <c r="B959" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="960" spans="1:2">
+      <c r="A960" t="s">
+        <v>3</v>
+      </c>
+      <c r="B960" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="961" spans="1:2">
+      <c r="A961" t="s">
+        <v>8</v>
+      </c>
+      <c r="B961" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="962" spans="1:2">
+      <c r="A962" t="s">
+        <v>423</v>
+      </c>
+      <c r="B962" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="963" spans="1:2">
+      <c r="A963" t="s">
+        <v>8</v>
+      </c>
+      <c r="B963" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="964" spans="1:2">
+      <c r="A964" t="s">
+        <v>1</v>
+      </c>
+      <c r="B964" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="965" spans="1:2">
+      <c r="A965" t="s">
+        <v>55</v>
+      </c>
+      <c r="B965" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="966" spans="1:2">
+      <c r="A966" t="s">
+        <v>3</v>
+      </c>
+      <c r="B966" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="967" spans="1:2">
+      <c r="A967" t="s">
+        <v>10</v>
+      </c>
+      <c r="B967" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="968" spans="1:2">
+      <c r="A968" t="s">
+        <v>3</v>
+      </c>
+      <c r="B968" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="969" spans="1:2">
+      <c r="A969" t="s">
+        <v>8</v>
+      </c>
+      <c r="B969" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="970" spans="1:2">
+      <c r="A970" t="s">
+        <v>3</v>
+      </c>
+      <c r="B970" t="s">
+        <v>997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>